<commit_message>
Refactor spreadsheet generator and add documentation
</commit_message>
<xml_diff>
--- a/mobile_security_checklist.xlsx
+++ b/mobile_security_checklist.xlsx
@@ -101,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -123,6 +123,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -605,200 +608,200 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="D1" s="11" t="inlineStr">
         <is>
           <t>Feature</t>
         </is>
       </c>
-      <c r="E1" s="10" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>Security requirement</t>
         </is>
       </c>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>Solution in app / Comments</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>Last updated</t>
         </is>
       </c>
-      <c r="H1" s="10" t="inlineStr">
+      <c r="H1" s="11" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="I1" s="10" t="inlineStr">
+      <c r="I1" s="11" t="inlineStr">
         <is>
           <t>Reference</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="inlineStr">
+      <c r="A2" s="12" t="inlineStr">
         <is>
           <t>SD.1</t>
         </is>
       </c>
-      <c r="B2" s="11" t="inlineStr">
+      <c r="B2" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C2" s="11" t="inlineStr">
+      <c r="C2" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D2" s="11" t="inlineStr">
+      <c r="D2" s="12" t="inlineStr">
         <is>
           <t>Login / Signup, keeping user session alive</t>
         </is>
       </c>
-      <c r="E2" s="11" t="inlineStr">
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>All tokens / credentials must be stored in keychain/keystore if they are persisted</t>
         </is>
       </c>
-      <c r="F2" s="11" t="inlineStr"/>
-      <c r="G2" s="12">
-        <f>IFERROR(A2+E2+"x",TODAY())</f>
+      <c r="F2" s="12" t="inlineStr"/>
+      <c r="G2" s="13">
+        <f>IFERROR(B2+F22+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H2" s="11" t="inlineStr">
+      <c r="H2" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I2" s="13" t="inlineStr">
+      <c r="I2" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="inlineStr">
+      <c r="A3" s="12" t="inlineStr">
         <is>
           <t>SD.2</t>
         </is>
       </c>
-      <c r="B3" s="11" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C3" s="11" t="inlineStr">
+      <c r="C3" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D3" s="11" t="inlineStr">
+      <c r="D3" s="12" t="inlineStr">
         <is>
           <t>Storing environment variables</t>
         </is>
       </c>
-      <c r="E3" s="11" t="inlineStr">
+      <c r="E3" s="12" t="inlineStr">
         <is>
           <t>Environment variables cannot be stored in github repository. All envs should be stored in secrets on CI (e. g. Bitrise)</t>
         </is>
       </c>
-      <c r="F3" s="11" t="inlineStr"/>
-      <c r="G3" s="12">
-        <f>IFERROR(A3+E3+"x",TODAY())</f>
+      <c r="F3" s="12" t="inlineStr"/>
+      <c r="G3" s="13">
+        <f>IFERROR(B3+F33+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H3" s="11" t="inlineStr">
+      <c r="H3" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I3" s="13" t="inlineStr">
+      <c r="I3" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="inlineStr">
+      <c r="A4" s="12" t="inlineStr">
         <is>
           <t>SD.3</t>
         </is>
       </c>
-      <c r="B4" s="11" t="inlineStr">
+      <c r="B4" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C4" s="11" t="inlineStr">
+      <c r="C4" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D4" s="11" t="inlineStr">
+      <c r="D4" s="12" t="inlineStr">
         <is>
           <t>App is using logs</t>
         </is>
       </c>
-      <c r="E4" s="11" t="inlineStr">
+      <c r="E4" s="12" t="inlineStr">
         <is>
           <t>No sensitive data is written to application logs</t>
         </is>
       </c>
-      <c r="F4" s="11" t="inlineStr"/>
-      <c r="G4" s="12">
-        <f>IFERROR(A4+E4+"x",TODAY())</f>
+      <c r="F4" s="12" t="inlineStr"/>
+      <c r="G4" s="13">
+        <f>IFERROR(B4+F44+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H4" s="11" t="inlineStr">
+      <c r="H4" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I4" s="13" t="inlineStr">
+      <c r="I4" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="inlineStr">
+      <c r="A5" s="12" t="inlineStr">
         <is>
           <t>SD.4</t>
         </is>
       </c>
-      <c r="B5" s="11" t="inlineStr">
+      <c r="B5" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C5" s="11" t="inlineStr">
+      <c r="C5" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D5" s="11" t="inlineStr">
+      <c r="D5" s="12" t="inlineStr">
         <is>
           <t>Sensitive aplication logic</t>
         </is>
       </c>
-      <c r="E5" s="11" t="inlineStr">
+      <c r="E5" s="12" t="inlineStr">
         <is>
           <t>Validate every update of a sensitive value with the server. 
  Do not validate sensitive features locally 
@@ -807,1404 +810,1404 @@
  - Coins for premium features</t>
         </is>
       </c>
-      <c r="F5" s="11" t="inlineStr"/>
-      <c r="G5" s="12">
-        <f>IFERROR(A5+E5+"x",TODAY())</f>
+      <c r="F5" s="12" t="inlineStr"/>
+      <c r="G5" s="13">
+        <f>IFERROR(B5+F55+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H5" s="11" t="inlineStr">
+      <c r="H5" s="12" t="inlineStr">
         <is>
           <t>Critical</t>
         </is>
       </c>
-      <c r="I5" s="13" t="inlineStr">
+      <c r="I5" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="A6" s="12" t="inlineStr">
         <is>
           <t>SD.5</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C6" s="11" t="inlineStr">
+      <c r="C6" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="12" t="inlineStr">
         <is>
           <t>Hardcoded keys</t>
         </is>
       </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>App doesn't store sensitive hardcoded keys inside app and conforms to best practices of storing hardcoded keys</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr"/>
-      <c r="G6" s="12">
-        <f>IFERROR(A6+E6+"x",TODAY())</f>
+      <c r="F6" s="12" t="inlineStr"/>
+      <c r="G6" s="13">
+        <f>IFERROR(B6+F66+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H6" s="12" t="inlineStr">
         <is>
           <t>Critical</t>
         </is>
       </c>
-      <c r="I6" s="13" t="inlineStr">
+      <c r="I6" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="inlineStr">
+      <c r="A7" s="12" t="inlineStr">
         <is>
           <t>SD.6</t>
         </is>
       </c>
-      <c r="B7" s="11" t="inlineStr">
+      <c r="B7" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C7" s="11" t="inlineStr">
+      <c r="C7" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D7" s="11" t="inlineStr">
+      <c r="D7" s="12" t="inlineStr">
         <is>
           <t>Login / signup</t>
         </is>
       </c>
-      <c r="E7" s="11" t="inlineStr">
+      <c r="E7" s="12" t="inlineStr">
         <is>
           <t>Do not store user password in local data storage</t>
         </is>
       </c>
-      <c r="F7" s="11" t="inlineStr"/>
-      <c r="G7" s="12">
-        <f>IFERROR(A7+E7+"x",TODAY())</f>
+      <c r="F7" s="12" t="inlineStr"/>
+      <c r="G7" s="13">
+        <f>IFERROR(B7+F77+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H7" s="11" t="inlineStr">
+      <c r="H7" s="12" t="inlineStr">
         <is>
           <t>Critical</t>
         </is>
       </c>
-      <c r="I7" s="13" t="inlineStr">
+      <c r="I7" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11" t="inlineStr">
+      <c r="A8" s="12" t="inlineStr">
         <is>
           <t>SD.7</t>
         </is>
       </c>
-      <c r="B8" s="11" t="inlineStr">
+      <c r="B8" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C8" s="11" t="inlineStr">
+      <c r="C8" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D8" s="11" t="inlineStr">
+      <c r="D8" s="12" t="inlineStr">
         <is>
           <t>Third party service with API keys</t>
         </is>
       </c>
-      <c r="E8" s="11" t="inlineStr">
+      <c r="E8" s="12" t="inlineStr">
         <is>
           <t>Keys generated in Third Party service like Google Cloud should have minimum set of permissions. 
  It should have assigned bundleID / AppID to key, It will accept data only from those apps</t>
         </is>
       </c>
-      <c r="F8" s="11" t="inlineStr"/>
-      <c r="G8" s="12">
-        <f>IFERROR(A8+E8+"x",TODAY())</f>
+      <c r="F8" s="12" t="inlineStr"/>
+      <c r="G8" s="13">
+        <f>IFERROR(B8+F88+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H8" s="11" t="inlineStr">
+      <c r="H8" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I8" s="13" t="inlineStr">
+      <c r="I8" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="inlineStr">
+      <c r="A9" s="12" t="inlineStr">
         <is>
           <t>SD.8</t>
         </is>
       </c>
-      <c r="B9" s="11" t="inlineStr">
+      <c r="B9" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C9" s="11" t="inlineStr">
+      <c r="C9" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D9" s="11" t="inlineStr">
+      <c r="D9" s="12" t="inlineStr">
         <is>
           <t>Authentication requires to enter data (password, pin) through e.g. keyboard</t>
         </is>
       </c>
-      <c r="E9" s="11" t="inlineStr">
+      <c r="E9" s="12" t="inlineStr">
         <is>
           <t>No sensitive data, such as passwords or pins, is exposed through the user interface. You have to use secure text entry for fields</t>
         </is>
       </c>
-      <c r="F9" s="11" t="inlineStr"/>
-      <c r="G9" s="12">
-        <f>IFERROR(A9+E9+"x",TODAY())</f>
+      <c r="F9" s="12" t="inlineStr"/>
+      <c r="G9" s="13">
+        <f>IFERROR(B9+F99+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H9" s="11" t="inlineStr">
+      <c r="H9" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I9" s="13" t="inlineStr">
+      <c r="I9" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="inlineStr">
+      <c r="A10" s="12" t="inlineStr">
         <is>
           <t>SD.9</t>
         </is>
       </c>
-      <c r="B10" s="11" t="inlineStr">
+      <c r="B10" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C10" s="11" t="inlineStr">
+      <c r="C10" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D10" s="11" t="inlineStr">
+      <c r="D10" s="12" t="inlineStr">
         <is>
           <t>App is making requests to REST API</t>
         </is>
       </c>
-      <c r="E10" s="11" t="inlineStr">
+      <c r="E10" s="12" t="inlineStr">
         <is>
           <t>Whole communication should use only HTTPS protocol</t>
         </is>
       </c>
-      <c r="F10" s="11" t="inlineStr"/>
-      <c r="G10" s="12">
-        <f>IFERROR(A10+E10+"x",TODAY())</f>
+      <c r="F10" s="12" t="inlineStr"/>
+      <c r="G10" s="13">
+        <f>IFERROR(B10+F1010+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H10" s="11" t="inlineStr">
+      <c r="H10" s="12" t="inlineStr">
         <is>
           <t>Critical</t>
         </is>
       </c>
-      <c r="I10" s="13" t="inlineStr">
+      <c r="I10" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="inlineStr">
+      <c r="A11" s="12" t="inlineStr">
         <is>
           <t>SD.10</t>
         </is>
       </c>
-      <c r="B11" s="11" t="inlineStr">
+      <c r="B11" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C11" s="11" t="inlineStr">
+      <c r="C11" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D11" s="11" t="inlineStr">
+      <c r="D11" s="12" t="inlineStr">
         <is>
           <t>Platforms with native obfuscation: Android, Flutter, React-Native</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
+      <c r="E11" s="12" t="inlineStr">
         <is>
           <t>Obfuscation should be configured. For Android: App should have proguard/r8 enabled</t>
         </is>
       </c>
-      <c r="F11" s="11" t="inlineStr"/>
-      <c r="G11" s="12">
-        <f>IFERROR(A11+E11+"x",TODAY())</f>
+      <c r="F11" s="12" t="inlineStr"/>
+      <c r="G11" s="13">
+        <f>IFERROR(B11+F1111+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H11" s="11" t="inlineStr">
+      <c r="H11" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I11" s="13" t="inlineStr">
+      <c r="I11" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="inlineStr">
+      <c r="A12" s="12" t="inlineStr">
         <is>
           <t>SD.11</t>
         </is>
       </c>
-      <c r="B12" s="11" t="inlineStr">
+      <c r="B12" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C12" s="11" t="inlineStr">
+      <c r="C12" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D12" s="11" t="inlineStr">
+      <c r="D12" s="12" t="inlineStr">
         <is>
           <t>App is adding new permissions</t>
         </is>
       </c>
-      <c r="E12" s="11" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
         <is>
           <t>Review permissions and use only necessary</t>
         </is>
       </c>
-      <c r="F12" s="11" t="inlineStr"/>
-      <c r="G12" s="12">
-        <f>IFERROR(A12+E12+"x",TODAY())</f>
+      <c r="F12" s="12" t="inlineStr"/>
+      <c r="G12" s="13">
+        <f>IFERROR(B12+F1212+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H12" s="11" t="inlineStr">
+      <c r="H12" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I12" s="13" t="inlineStr">
+      <c r="I12" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="inlineStr">
+      <c r="A13" s="12" t="inlineStr">
         <is>
           <t>SD.12</t>
         </is>
       </c>
-      <c r="B13" s="11" t="inlineStr">
+      <c r="B13" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C13" s="11" t="inlineStr">
+      <c r="C13" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D13" s="11" t="inlineStr">
+      <c r="D13" s="12" t="inlineStr">
         <is>
           <t>App has apple certificates, google keystore or other sensitive files</t>
         </is>
       </c>
-      <c r="E13" s="11" t="inlineStr">
+      <c r="E13" s="12" t="inlineStr">
         <is>
           <t>Secure them in proper place and describe how it's achieved. E.g. make sure they are all stored only in 1pass and access has minimal amount of people</t>
         </is>
       </c>
-      <c r="F13" s="11" t="inlineStr"/>
-      <c r="G13" s="12">
-        <f>IFERROR(A13+E13+"x",TODAY())</f>
+      <c r="F13" s="12" t="inlineStr"/>
+      <c r="G13" s="13">
+        <f>IFERROR(B13+F1313+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H13" s="11" t="inlineStr">
+      <c r="H13" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I13" s="13" t="inlineStr">
+      <c r="I13" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="inlineStr">
+      <c r="A14" s="12" t="inlineStr">
         <is>
           <t>SD.13</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
+      <c r="B14" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C14" s="11" t="inlineStr">
+      <c r="C14" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
+      <c r="D14" s="12" t="inlineStr">
         <is>
           <t>App is persisting data. App saves files</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E14" s="12" t="inlineStr">
         <is>
           <t>No sensitive data is included in backups generated by the mobile operating system. Make sure that all files are saved in proper place</t>
         </is>
       </c>
-      <c r="F14" s="11" t="inlineStr"/>
-      <c r="G14" s="12">
-        <f>IFERROR(A14+E14+"x",TODAY())</f>
+      <c r="F14" s="12" t="inlineStr"/>
+      <c r="G14" s="13">
+        <f>IFERROR(B14+F1414+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H14" s="11" t="inlineStr">
+      <c r="H14" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I14" s="13" t="inlineStr">
+      <c r="I14" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="inlineStr">
+      <c r="A15" s="12" t="inlineStr">
         <is>
           <t>SD.14</t>
         </is>
       </c>
-      <c r="B15" s="11" t="inlineStr">
+      <c r="B15" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C15" s="11" t="inlineStr">
+      <c r="C15" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D15" s="11" t="inlineStr">
+      <c r="D15" s="12" t="inlineStr">
         <is>
           <t>User can recover account</t>
         </is>
       </c>
-      <c r="E15" s="11" t="inlineStr">
+      <c r="E15" s="12" t="inlineStr">
         <is>
           <t>The app doesn't rely on a single insecure communication channel (email or SMS) for critical operations, such as enrollments and account recovery. You should have possiblity to verify somehow user identity e.g. security questions, additional informtation about what happend in account</t>
         </is>
       </c>
-      <c r="F15" s="11" t="inlineStr"/>
-      <c r="G15" s="12">
-        <f>IFERROR(A15+E15+"x",TODAY())</f>
+      <c r="F15" s="12" t="inlineStr"/>
+      <c r="G15" s="13">
+        <f>IFERROR(B15+F1515+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H15" s="11" t="inlineStr">
+      <c r="H15" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I15" s="13" t="inlineStr">
+      <c r="I15" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="inlineStr">
+      <c r="A16" s="12" t="inlineStr">
         <is>
           <t>SD.15</t>
         </is>
       </c>
-      <c r="B16" s="11" t="inlineStr">
+      <c r="B16" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C16" s="11" t="inlineStr">
+      <c r="C16" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D16" s="11" t="inlineStr">
+      <c r="D16" s="12" t="inlineStr">
         <is>
           <t>URLs passed outside of app (for example from API)</t>
         </is>
       </c>
-      <c r="E16" s="11" t="inlineStr">
+      <c r="E16" s="12" t="inlineStr">
         <is>
           <t>Validate url according whitelist of urls within app</t>
         </is>
       </c>
-      <c r="F16" s="11" t="inlineStr"/>
-      <c r="G16" s="12">
-        <f>IFERROR(A16+E16+"x",TODAY())</f>
+      <c r="F16" s="12" t="inlineStr"/>
+      <c r="G16" s="13">
+        <f>IFERROR(B16+F1616+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H16" s="11" t="inlineStr">
+      <c r="H16" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I16" s="13" t="inlineStr">
+      <c r="I16" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="inlineStr">
+      <c r="A17" s="12" t="inlineStr">
         <is>
           <t>SD.16</t>
         </is>
       </c>
-      <c r="B17" s="11" t="inlineStr">
+      <c r="B17" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C17" s="11" t="inlineStr">
+      <c r="C17" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D17" s="11" t="inlineStr">
+      <c r="D17" s="12" t="inlineStr">
         <is>
           <t>Login / signup</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
+      <c r="E17" s="12" t="inlineStr">
         <is>
           <t>Removing all data after logout, keychain, files, cache</t>
         </is>
       </c>
-      <c r="F17" s="11" t="inlineStr"/>
-      <c r="G17" s="12">
-        <f>IFERROR(A17+E17+"x",TODAY())</f>
+      <c r="F17" s="12" t="inlineStr"/>
+      <c r="G17" s="13">
+        <f>IFERROR(B17+F1717+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H17" s="11" t="inlineStr">
+      <c r="H17" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I17" s="13" t="inlineStr">
+      <c r="I17" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="inlineStr">
+      <c r="A18" s="12" t="inlineStr">
         <is>
           <t>SD.17</t>
         </is>
       </c>
-      <c r="B18" s="11" t="inlineStr">
+      <c r="B18" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C18" s="11" t="inlineStr">
+      <c r="C18" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D18" s="11" t="inlineStr">
+      <c r="D18" s="12" t="inlineStr">
         <is>
           <t>User enter sensitive data or password into inputs</t>
         </is>
       </c>
-      <c r="E18" s="11" t="inlineStr">
+      <c r="E18" s="12" t="inlineStr">
         <is>
           <t>Disable additional hardware keyboard connected to device, user can only use fabric one</t>
         </is>
       </c>
-      <c r="F18" s="11" t="inlineStr"/>
-      <c r="G18" s="12">
-        <f>IFERROR(A18+E18+"x",TODAY())</f>
+      <c r="F18" s="12" t="inlineStr"/>
+      <c r="G18" s="13">
+        <f>IFERROR(B18+F1818+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H18" s="11" t="inlineStr">
+      <c r="H18" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I18" s="13" t="inlineStr">
+      <c r="I18" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="inlineStr">
+      <c r="A19" s="12" t="inlineStr">
         <is>
           <t>SD.18</t>
         </is>
       </c>
-      <c r="B19" s="11" t="inlineStr">
+      <c r="B19" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C19" s="11" t="inlineStr">
+      <c r="C19" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="D19" s="11" t="inlineStr">
+      <c r="D19" s="12" t="inlineStr">
         <is>
           <t>Logout</t>
         </is>
       </c>
-      <c r="E19" s="11" t="inlineStr">
+      <c r="E19" s="12" t="inlineStr">
         <is>
           <t>Invalidate access token through request to backend</t>
         </is>
       </c>
-      <c r="F19" s="11" t="inlineStr"/>
-      <c r="G19" s="12">
-        <f>IFERROR(A19+E19+"x",TODAY())</f>
+      <c r="F19" s="12" t="inlineStr"/>
+      <c r="G19" s="13">
+        <f>IFERROR(B19+F1919+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H19" s="11" t="inlineStr">
+      <c r="H19" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I19" s="13" t="inlineStr">
+      <c r="I19" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="inlineStr">
+      <c r="A20" s="12" t="inlineStr">
         <is>
           <t>SE.1</t>
         </is>
       </c>
-      <c r="B20" s="11" t="inlineStr">
+      <c r="B20" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C20" s="11" t="inlineStr">
+      <c r="C20" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D20" s="11" t="inlineStr">
+      <c r="D20" s="12" t="inlineStr">
         <is>
           <t>Fintech app or very sensitive application</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
+      <c r="E20" s="12" t="inlineStr">
         <is>
           <t>To increase security of the application it could be additionally protected with PIN screen</t>
         </is>
       </c>
-      <c r="F20" s="11" t="inlineStr"/>
-      <c r="G20" s="12">
-        <f>IFERROR(A20+E20+"x",TODAY())</f>
+      <c r="F20" s="12" t="inlineStr"/>
+      <c r="G20" s="13">
+        <f>IFERROR(B20+F2020+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H20" s="11" t="inlineStr">
+      <c r="H20" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I20" s="13" t="inlineStr">
+      <c r="I20" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="inlineStr">
+      <c r="A21" s="12" t="inlineStr">
         <is>
           <t>SE.2</t>
         </is>
       </c>
-      <c r="B21" s="11" t="inlineStr">
+      <c r="B21" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C21" s="11" t="inlineStr">
+      <c r="C21" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D21" s="11" t="inlineStr">
+      <c r="D21" s="12" t="inlineStr">
         <is>
           <t>User shouldn't use jailbroken/rooted device</t>
         </is>
       </c>
-      <c r="E21" s="11" t="inlineStr">
+      <c r="E21" s="12" t="inlineStr">
         <is>
           <t>The app detects and reacts to the presence of a rooted or jailbroken device either by alerting the user or terminating the app</t>
         </is>
       </c>
-      <c r="F21" s="11" t="inlineStr"/>
-      <c r="G21" s="12">
-        <f>IFERROR(A21+E21+"x",TODAY())</f>
+      <c r="F21" s="12" t="inlineStr"/>
+      <c r="G21" s="13">
+        <f>IFERROR(B21+F2121+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H21" s="11" t="inlineStr">
+      <c r="H21" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I21" s="13" t="inlineStr">
+      <c r="I21" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="11" t="inlineStr">
+      <c r="A22" s="12" t="inlineStr">
         <is>
           <t>SE.3</t>
         </is>
       </c>
-      <c r="B22" s="11" t="inlineStr">
+      <c r="B22" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C22" s="11" t="inlineStr">
+      <c r="C22" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D22" s="11" t="inlineStr">
+      <c r="D22" s="12" t="inlineStr">
         <is>
           <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
         </is>
       </c>
-      <c r="E22" s="11" t="inlineStr">
+      <c r="E22" s="12" t="inlineStr">
         <is>
           <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
         </is>
       </c>
-      <c r="F22" s="11" t="inlineStr"/>
-      <c r="G22" s="12">
-        <f>IFERROR(A22+E22+"x",TODAY())</f>
+      <c r="F22" s="12" t="inlineStr"/>
+      <c r="G22" s="13">
+        <f>IFERROR(B22+F2222+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H22" s="11" t="inlineStr">
+      <c r="H22" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I22" s="13" t="inlineStr">
+      <c r="I22" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="11" t="inlineStr">
+      <c r="A23" s="12" t="inlineStr">
         <is>
           <t>SE.4</t>
         </is>
       </c>
-      <c r="B23" s="11" t="inlineStr">
+      <c r="B23" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C23" s="11" t="inlineStr">
+      <c r="C23" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D23" s="11" t="inlineStr">
+      <c r="D23" s="12" t="inlineStr">
         <is>
           <t>The app catches and handles possible exceptions</t>
         </is>
       </c>
-      <c r="E23" s="11" t="inlineStr">
+      <c r="E23" s="12" t="inlineStr">
         <is>
           <t>Make sure you have added sentry, bugsnag or crashlitics or other to catch all crashes</t>
         </is>
       </c>
-      <c r="F23" s="11" t="inlineStr"/>
-      <c r="G23" s="12">
-        <f>IFERROR(A23+E23+"x",TODAY())</f>
+      <c r="F23" s="12" t="inlineStr"/>
+      <c r="G23" s="13">
+        <f>IFERROR(B23+F2323+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H23" s="11" t="inlineStr">
+      <c r="H23" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I23" s="13" t="inlineStr">
+      <c r="I23" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="11" t="inlineStr">
+      <c r="A24" s="12" t="inlineStr">
         <is>
           <t>SE.5</t>
         </is>
       </c>
-      <c r="B24" s="11" t="inlineStr">
+      <c r="B24" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C24" s="11" t="inlineStr">
+      <c r="C24" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D24" s="11" t="inlineStr">
+      <c r="D24" s="12" t="inlineStr">
         <is>
           <t>Storing data using hashes</t>
         </is>
       </c>
-      <c r="E24" s="11" t="inlineStr">
+      <c r="E24" s="12" t="inlineStr">
         <is>
           <t>Hashed data should use unique (for every user) salt to increase the complexity of reversing the operation</t>
         </is>
       </c>
-      <c r="F24" s="11" t="inlineStr"/>
-      <c r="G24" s="12">
-        <f>IFERROR(A24+E24+"x",TODAY())</f>
+      <c r="F24" s="12" t="inlineStr"/>
+      <c r="G24" s="13">
+        <f>IFERROR(B24+F2424+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H24" s="11" t="inlineStr">
+      <c r="H24" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I24" s="13" t="inlineStr">
+      <c r="I24" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="11" t="inlineStr">
+      <c r="A25" s="12" t="inlineStr">
         <is>
           <t>SE.6</t>
         </is>
       </c>
-      <c r="B25" s="11" t="inlineStr">
+      <c r="B25" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C25" s="11" t="inlineStr">
+      <c r="C25" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D25" s="11" t="inlineStr">
+      <c r="D25" s="12" t="inlineStr">
         <is>
           <t>Very sensitive applications like banking apps</t>
         </is>
       </c>
-      <c r="E25" s="11" t="inlineStr">
+      <c r="E25" s="12" t="inlineStr">
         <is>
           <t>Two factor authentication</t>
         </is>
       </c>
-      <c r="F25" s="11" t="inlineStr"/>
-      <c r="G25" s="12">
-        <f>IFERROR(A25+E25+"x",TODAY())</f>
+      <c r="F25" s="12" t="inlineStr"/>
+      <c r="G25" s="13">
+        <f>IFERROR(B25+F2525+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H25" s="11" t="inlineStr">
+      <c r="H25" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I25" s="13" t="inlineStr">
+      <c r="I25" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="11" t="inlineStr">
+      <c r="A26" s="12" t="inlineStr">
         <is>
           <t>SE.7</t>
         </is>
       </c>
-      <c r="B26" s="11" t="inlineStr">
+      <c r="B26" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C26" s="11" t="inlineStr">
+      <c r="C26" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D26" s="11" t="inlineStr">
+      <c r="D26" s="12" t="inlineStr">
         <is>
           <t>App is recognizing device as trust device</t>
         </is>
       </c>
-      <c r="E26" s="11" t="inlineStr">
+      <c r="E26" s="12" t="inlineStr">
         <is>
           <t>The app implements a 'device binding' functionality using a device fingerprint derived from multiple properties unique to the device</t>
         </is>
       </c>
-      <c r="F26" s="11" t="inlineStr"/>
-      <c r="G26" s="12">
-        <f>IFERROR(A26+E26+"x",TODAY())</f>
+      <c r="F26" s="12" t="inlineStr"/>
+      <c r="G26" s="13">
+        <f>IFERROR(B26+F2626+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H26" s="11" t="inlineStr">
+      <c r="H26" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I26" s="13" t="inlineStr">
+      <c r="I26" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="11" t="inlineStr">
+      <c r="A27" s="12" t="inlineStr">
         <is>
           <t>SE.8</t>
         </is>
       </c>
-      <c r="B27" s="11" t="inlineStr">
+      <c r="B27" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C27" s="11" t="inlineStr">
+      <c r="C27" s="12" t="inlineStr">
         <is>
           <t>Extra</t>
         </is>
       </c>
-      <c r="D27" s="11" t="inlineStr">
+      <c r="D27" s="12" t="inlineStr">
         <is>
           <t>Login</t>
         </is>
       </c>
-      <c r="E27" s="11" t="inlineStr">
+      <c r="E27" s="12" t="inlineStr">
         <is>
           <t>Block App after number of login failures</t>
         </is>
       </c>
-      <c r="F27" s="11" t="inlineStr"/>
-      <c r="G27" s="12">
-        <f>IFERROR(A27+E27+"x",TODAY())</f>
+      <c r="F27" s="12" t="inlineStr"/>
+      <c r="G27" s="13">
+        <f>IFERROR(B27+F2727+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H27" s="11" t="inlineStr">
+      <c r="H27" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I27" s="13" t="inlineStr">
+      <c r="I27" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="11" t="inlineStr">
+      <c r="A28" s="12" t="inlineStr">
         <is>
           <t>SW.1</t>
         </is>
       </c>
-      <c r="B28" s="11" t="inlineStr">
+      <c r="B28" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C28" s="11" t="inlineStr">
+      <c r="C28" s="12" t="inlineStr">
         <is>
           <t>WebView</t>
         </is>
       </c>
-      <c r="D28" s="11" t="inlineStr">
+      <c r="D28" s="12" t="inlineStr">
         <is>
           <t>App is using webview</t>
         </is>
       </c>
-      <c r="E28" s="11" t="inlineStr">
+      <c r="E28" s="12" t="inlineStr">
         <is>
           <t>JavaScript is disabled in WebViews unless explicitly required</t>
         </is>
       </c>
-      <c r="F28" s="11" t="inlineStr"/>
-      <c r="G28" s="12">
-        <f>IFERROR(A28+E28+"x",TODAY())</f>
+      <c r="F28" s="12" t="inlineStr"/>
+      <c r="G28" s="13">
+        <f>IFERROR(B28+F2828+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H28" s="11" t="inlineStr">
+      <c r="H28" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I28" s="13" t="inlineStr">
+      <c r="I28" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="11" t="inlineStr">
+      <c r="A29" s="12" t="inlineStr">
         <is>
           <t>SU.1</t>
         </is>
       </c>
-      <c r="B29" s="11" t="inlineStr">
+      <c r="B29" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C29" s="11" t="inlineStr">
+      <c r="C29" s="12" t="inlineStr">
         <is>
           <t>Upload</t>
         </is>
       </c>
-      <c r="D29" s="11" t="inlineStr">
+      <c r="D29" s="12" t="inlineStr">
         <is>
           <t>App has file upload</t>
         </is>
       </c>
-      <c r="E29" s="11" t="inlineStr">
+      <c r="E29" s="12" t="inlineStr">
         <is>
           <t>Limit maximum number of files that can be uploaded at once</t>
         </is>
       </c>
-      <c r="F29" s="11" t="inlineStr"/>
-      <c r="G29" s="12">
-        <f>IFERROR(A29+E29+"x",TODAY())</f>
+      <c r="F29" s="12" t="inlineStr"/>
+      <c r="G29" s="13">
+        <f>IFERROR(B29+F2929+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H29" s="11" t="inlineStr">
+      <c r="H29" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I29" s="13" t="inlineStr">
+      <c r="I29" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="11" t="inlineStr">
+      <c r="A30" s="12" t="inlineStr">
         <is>
           <t>SG.1</t>
         </is>
       </c>
-      <c r="B30" s="11" t="inlineStr">
+      <c r="B30" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C30" s="11" t="inlineStr">
+      <c r="C30" s="12" t="inlineStr">
         <is>
           <t>GDPR</t>
         </is>
       </c>
-      <c r="D30" s="11" t="inlineStr">
+      <c r="D30" s="12" t="inlineStr">
         <is>
           <t>Persising user personal information (name, phone, email, ...) on the device</t>
         </is>
       </c>
-      <c r="E30" s="11" t="inlineStr">
+      <c r="E30" s="12" t="inlineStr">
         <is>
           <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
         </is>
       </c>
-      <c r="F30" s="11" t="inlineStr"/>
-      <c r="G30" s="12">
-        <f>IFERROR(A30+E30+"x",TODAY())</f>
+      <c r="F30" s="12" t="inlineStr"/>
+      <c r="G30" s="13">
+        <f>IFERROR(B30+F3030+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H30" s="11" t="inlineStr">
+      <c r="H30" s="12" t="inlineStr">
         <is>
           <t>Critical</t>
         </is>
       </c>
-      <c r="I30" s="13" t="inlineStr">
+      <c r="I30" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="11" t="inlineStr">
+      <c r="A31" s="12" t="inlineStr">
         <is>
           <t>SG.2</t>
         </is>
       </c>
-      <c r="B31" s="11" t="inlineStr">
+      <c r="B31" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C31" s="11" t="inlineStr">
+      <c r="C31" s="12" t="inlineStr">
         <is>
           <t>GDPR</t>
         </is>
       </c>
-      <c r="D31" s="11" t="inlineStr">
+      <c r="D31" s="12" t="inlineStr">
         <is>
           <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
         </is>
       </c>
-      <c r="E31" s="11" t="inlineStr">
+      <c r="E31" s="12" t="inlineStr">
         <is>
           <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
         </is>
       </c>
-      <c r="F31" s="11" t="inlineStr"/>
-      <c r="G31" s="12">
-        <f>IFERROR(A31+E31+"x",TODAY())</f>
+      <c r="F31" s="12" t="inlineStr"/>
+      <c r="G31" s="13">
+        <f>IFERROR(B31+F3131+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H31" s="11" t="inlineStr">
+      <c r="H31" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I31" s="13" t="inlineStr">
+      <c r="I31" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="11" t="inlineStr">
+      <c r="A32" s="12" t="inlineStr">
         <is>
           <t>SG.3</t>
         </is>
       </c>
-      <c r="B32" s="11" t="inlineStr">
+      <c r="B32" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C32" s="11" t="inlineStr">
+      <c r="C32" s="12" t="inlineStr">
         <is>
           <t>GDPR</t>
         </is>
       </c>
-      <c r="D32" s="11" t="inlineStr">
+      <c r="D32" s="12" t="inlineStr">
         <is>
           <t>Sending personal data outside of the application</t>
         </is>
       </c>
-      <c r="E32" s="11" t="inlineStr">
+      <c r="E32" s="12" t="inlineStr">
         <is>
           <t>All requests must be authenticated</t>
         </is>
       </c>
-      <c r="F32" s="11" t="inlineStr"/>
-      <c r="G32" s="12">
-        <f>IFERROR(A32+E32+"x",TODAY())</f>
+      <c r="F32" s="12" t="inlineStr"/>
+      <c r="G32" s="13">
+        <f>IFERROR(B32+F3232+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H32" s="11" t="inlineStr">
+      <c r="H32" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I32" s="13" t="inlineStr">
+      <c r="I32" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="11" t="inlineStr">
+      <c r="A33" s="12" t="inlineStr">
         <is>
           <t>SG.4</t>
         </is>
       </c>
-      <c r="B33" s="11" t="inlineStr">
+      <c r="B33" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C33" s="11" t="inlineStr">
+      <c r="C33" s="12" t="inlineStr">
         <is>
           <t>GDPR</t>
         </is>
       </c>
-      <c r="D33" s="11" t="inlineStr">
+      <c r="D33" s="12" t="inlineStr">
         <is>
           <t>Transferin personal data through REST API</t>
         </is>
       </c>
-      <c r="E33" s="11" t="inlineStr">
+      <c r="E33" s="12" t="inlineStr">
         <is>
           <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
         </is>
       </c>
-      <c r="F33" s="11" t="inlineStr"/>
-      <c r="G33" s="12">
-        <f>IFERROR(A33+E33+"x",TODAY())</f>
+      <c r="F33" s="12" t="inlineStr"/>
+      <c r="G33" s="13">
+        <f>IFERROR(B33+F3333+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H33" s="11" t="inlineStr">
+      <c r="H33" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I33" s="13" t="inlineStr">
+      <c r="I33" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="11" t="inlineStr">
+      <c r="A34" s="12" t="inlineStr">
         <is>
           <t>SG.5</t>
         </is>
       </c>
-      <c r="B34" s="11" t="inlineStr">
+      <c r="B34" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C34" s="11" t="inlineStr">
+      <c r="C34" s="12" t="inlineStr">
         <is>
           <t>GDPR</t>
         </is>
       </c>
-      <c r="D34" s="11" t="inlineStr">
+      <c r="D34" s="12" t="inlineStr">
         <is>
           <t>Displaying privacy policy screen during registration process</t>
         </is>
       </c>
-      <c r="E34" s="11" t="inlineStr">
+      <c r="E34" s="12" t="inlineStr">
         <is>
           <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
         </is>
       </c>
-      <c r="F34" s="11" t="inlineStr"/>
-      <c r="G34" s="12">
-        <f>IFERROR(A34+E34+"x",TODAY())</f>
+      <c r="F34" s="12" t="inlineStr"/>
+      <c r="G34" s="13">
+        <f>IFERROR(B34+F3434+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H34" s="11" t="inlineStr">
+      <c r="H34" s="12" t="inlineStr">
         <is>
           <t>Critical</t>
         </is>
       </c>
-      <c r="I34" s="13" t="inlineStr">
+      <c r="I34" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="11" t="inlineStr">
+      <c r="A35" s="12" t="inlineStr">
         <is>
           <t>SG.6</t>
         </is>
       </c>
-      <c r="B35" s="11" t="inlineStr">
+      <c r="B35" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C35" s="11" t="inlineStr">
+      <c r="C35" s="12" t="inlineStr">
         <is>
           <t>GDPR</t>
         </is>
       </c>
-      <c r="D35" s="11" t="inlineStr">
+      <c r="D35" s="12" t="inlineStr">
         <is>
           <t>Using non-production environments</t>
         </is>
       </c>
-      <c r="E35" s="11" t="inlineStr">
+      <c r="E35" s="12" t="inlineStr">
         <is>
           <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
         </is>
       </c>
-      <c r="F35" s="11" t="inlineStr"/>
-      <c r="G35" s="12">
-        <f>IFERROR(A35+E35+"x",TODAY())</f>
+      <c r="F35" s="12" t="inlineStr"/>
+      <c r="G35" s="13">
+        <f>IFERROR(B35+F3535+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H35" s="11" t="inlineStr">
+      <c r="H35" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I35" s="13" t="inlineStr">
+      <c r="I35" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="11" t="inlineStr">
+      <c r="A36" s="12" t="inlineStr">
         <is>
           <t>SEM.1</t>
         </is>
       </c>
-      <c r="B36" s="11" t="inlineStr">
+      <c r="B36" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C36" s="11" t="inlineStr">
+      <c r="C36" s="12" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D36" s="11" t="inlineStr">
+      <c r="D36" s="12" t="inlineStr">
         <is>
           <t>Application has input for user email address</t>
         </is>
       </c>
-      <c r="E36" s="11" t="inlineStr">
+      <c r="E36" s="12" t="inlineStr">
         <is>
           <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
         </is>
       </c>
-      <c r="F36" s="11" t="inlineStr"/>
-      <c r="G36" s="12">
-        <f>IFERROR(A36+E36+"x",TODAY())</f>
+      <c r="F36" s="12" t="inlineStr"/>
+      <c r="G36" s="13">
+        <f>IFERROR(B36+F3636+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H36" s="11" t="inlineStr">
+      <c r="H36" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I36" s="13" t="inlineStr">
+      <c r="I36" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="11" t="inlineStr">
+      <c r="A37" s="12" t="inlineStr">
         <is>
           <t>SV.1</t>
         </is>
       </c>
-      <c r="B37" s="11" t="inlineStr">
+      <c r="B37" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C37" s="11" t="inlineStr">
+      <c r="C37" s="12" t="inlineStr">
         <is>
           <t>Video</t>
         </is>
       </c>
-      <c r="D37" s="11" t="inlineStr">
+      <c r="D37" s="12" t="inlineStr">
         <is>
           <t>User can play video in the application</t>
         </is>
       </c>
-      <c r="E37" s="11" t="inlineStr">
+      <c r="E37" s="12" t="inlineStr">
         <is>
           <t>Video data must be received through HTTPS protocol</t>
         </is>
       </c>
-      <c r="F37" s="11" t="inlineStr"/>
-      <c r="G37" s="12">
-        <f>IFERROR(A37+E37+"x",TODAY())</f>
+      <c r="F37" s="12" t="inlineStr"/>
+      <c r="G37" s="13">
+        <f>IFERROR(B37+F3737+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H37" s="11" t="inlineStr">
+      <c r="H37" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I37" s="13" t="inlineStr">
+      <c r="I37" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="11" t="inlineStr">
+      <c r="A38" s="12" t="inlineStr">
         <is>
           <t>SL.1</t>
         </is>
       </c>
-      <c r="B38" s="11" t="inlineStr">
+      <c r="B38" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C38" s="11" t="inlineStr">
+      <c r="C38" s="12" t="inlineStr">
         <is>
           <t>Location</t>
         </is>
       </c>
-      <c r="D38" s="11" t="inlineStr">
+      <c r="D38" s="12" t="inlineStr">
         <is>
           <t>App is using location services</t>
         </is>
       </c>
-      <c r="E38" s="11" t="inlineStr">
+      <c r="E38" s="12" t="inlineStr">
         <is>
           <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
         </is>
       </c>
-      <c r="F38" s="11" t="inlineStr"/>
-      <c r="G38" s="12">
-        <f>IFERROR(A38+E38+"x",TODAY())</f>
+      <c r="F38" s="12" t="inlineStr"/>
+      <c r="G38" s="13">
+        <f>IFERROR(B38+F3838+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H38" s="11" t="inlineStr">
+      <c r="H38" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I38" s="13" t="inlineStr">
+      <c r="I38" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
@@ -2304,260 +2307,260 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="D1" s="11" t="inlineStr">
         <is>
           <t>Feature</t>
         </is>
       </c>
-      <c r="E1" s="10" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>Security requirement</t>
         </is>
       </c>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>Solution in app / Comments</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>Last updated</t>
         </is>
       </c>
-      <c r="H1" s="10" t="inlineStr">
+      <c r="H1" s="11" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="I1" s="10" t="inlineStr">
+      <c r="I1" s="11" t="inlineStr">
         <is>
           <t>Reference</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="inlineStr">
+      <c r="A2" s="12" t="inlineStr">
         <is>
           <t>iOS.1</t>
         </is>
       </c>
-      <c r="B2" s="11" t="inlineStr">
+      <c r="B2" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C2" s="11" t="inlineStr">
+      <c r="C2" s="12" t="inlineStr">
         <is>
           <t>iOS</t>
         </is>
       </c>
-      <c r="D2" s="11" t="inlineStr">
+      <c r="D2" s="12" t="inlineStr">
         <is>
           <t>Using UITextField with sensitive data</t>
         </is>
       </c>
-      <c r="E2" s="11" t="inlineStr">
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>Set autocorrectionType to .none in Sensitive UITextFields</t>
         </is>
       </c>
-      <c r="F2" s="11" t="inlineStr"/>
-      <c r="G2" s="12">
-        <f>IFERROR(A2+E2+"x",TODAY())</f>
+      <c r="F2" s="12" t="inlineStr"/>
+      <c r="G2" s="13">
+        <f>IFERROR(B2+F22+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H2" s="11" t="inlineStr">
+      <c r="H2" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I2" s="13" t="inlineStr">
+      <c r="I2" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="inlineStr">
+      <c r="A3" s="12" t="inlineStr">
         <is>
           <t>iOS.2</t>
         </is>
       </c>
-      <c r="B3" s="11" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C3" s="11" t="inlineStr">
+      <c r="C3" s="12" t="inlineStr">
         <is>
           <t>iOS</t>
         </is>
       </c>
-      <c r="D3" s="11" t="inlineStr">
+      <c r="D3" s="12" t="inlineStr">
         <is>
           <t>Using NSURLSession</t>
         </is>
       </c>
-      <c r="E3" s="11" t="inlineStr">
+      <c r="E3" s="12" t="inlineStr">
         <is>
           <t>By default NSURLSession stores data, such as HTTP requests and responses in the Cache.db database. 
  It should be disabled in URLSession with setting .ephemeral type instead of default one</t>
         </is>
       </c>
-      <c r="F3" s="11" t="inlineStr"/>
-      <c r="G3" s="12">
-        <f>IFERROR(A3+E3+"x",TODAY())</f>
+      <c r="F3" s="12" t="inlineStr"/>
+      <c r="G3" s="13">
+        <f>IFERROR(B3+F33+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H3" s="11" t="inlineStr">
+      <c r="H3" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I3" s="13" t="inlineStr">
+      <c r="I3" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="inlineStr">
+      <c r="A4" s="12" t="inlineStr">
         <is>
           <t>iOS.3</t>
         </is>
       </c>
-      <c r="B4" s="11" t="inlineStr">
+      <c r="B4" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C4" s="11" t="inlineStr">
+      <c r="C4" s="12" t="inlineStr">
         <is>
           <t>iOS</t>
         </is>
       </c>
-      <c r="D4" s="11" t="inlineStr">
+      <c r="D4" s="12" t="inlineStr">
         <is>
           <t>Certificate Pinning implemetation using TrustKit</t>
         </is>
       </c>
-      <c r="E4" s="11" t="inlineStr">
+      <c r="E4" s="12" t="inlineStr">
         <is>
           <t>Set kTSKDisableDefaultReportUri to true 
  By default this flag is false, which means it will be sending error reports to tool owner</t>
         </is>
       </c>
-      <c r="F4" s="11" t="inlineStr"/>
-      <c r="G4" s="12">
-        <f>IFERROR(A4+E4+"x",TODAY())</f>
+      <c r="F4" s="12" t="inlineStr"/>
+      <c r="G4" s="13">
+        <f>IFERROR(B4+F44+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H4" s="11" t="inlineStr">
+      <c r="H4" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I4" s="13" t="inlineStr">
+      <c r="I4" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="inlineStr">
+      <c r="A5" s="12" t="inlineStr">
         <is>
           <t>iOS.4</t>
         </is>
       </c>
-      <c r="B5" s="11" t="inlineStr">
+      <c r="B5" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C5" s="11" t="inlineStr">
+      <c r="C5" s="12" t="inlineStr">
         <is>
           <t>iOS</t>
         </is>
       </c>
-      <c r="D5" s="11" t="inlineStr">
+      <c r="D5" s="12" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
-      <c r="E5" s="11" t="inlineStr">
+      <c r="E5" s="12" t="inlineStr">
         <is>
           <t>Verify if not needed files are not included in the bundle. 
  Exclude them if needed using EXCLUDED_SOURCE_FILE_NAMES</t>
         </is>
       </c>
-      <c r="F5" s="11" t="inlineStr"/>
-      <c r="G5" s="12">
-        <f>IFERROR(A5+E5+"x",TODAY())</f>
+      <c r="F5" s="12" t="inlineStr"/>
+      <c r="G5" s="13">
+        <f>IFERROR(B5+F55+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H5" s="11" t="inlineStr">
+      <c r="H5" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I5" s="13" t="inlineStr">
+      <c r="I5" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="A6" s="12" t="inlineStr">
         <is>
           <t>iOS.5</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C6" s="11" t="inlineStr">
+      <c r="C6" s="12" t="inlineStr">
         <is>
           <t>iOS</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
+      <c r="D6" s="12" t="inlineStr">
         <is>
           <t>User enter sensitive data or password into inputs</t>
         </is>
       </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
         <is>
           <t>Verify that the app prevents usage of custom third-party keyboards whenever sensitive data is entered</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr"/>
-      <c r="G6" s="12">
-        <f>IFERROR(A6+E6+"x",TODAY())</f>
+      <c r="F6" s="12" t="inlineStr"/>
+      <c r="G6" s="13">
+        <f>IFERROR(B6+F66+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H6" s="11" t="inlineStr">
+      <c r="H6" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I6" s="13" t="inlineStr">
+      <c r="I6" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
@@ -2625,177 +2628,177 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="D1" s="10" t="inlineStr">
+      <c r="D1" s="11" t="inlineStr">
         <is>
           <t>Feature</t>
         </is>
       </c>
-      <c r="E1" s="10" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>Security requirement</t>
         </is>
       </c>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>Solution in app / Comments</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>Last updated</t>
         </is>
       </c>
-      <c r="H1" s="10" t="inlineStr">
+      <c r="H1" s="11" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="I1" s="10" t="inlineStr">
+      <c r="I1" s="11" t="inlineStr">
         <is>
           <t>Reference</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="inlineStr">
+      <c r="A2" s="12" t="inlineStr">
         <is>
           <t>AND.1</t>
         </is>
       </c>
-      <c r="B2" s="11" t="inlineStr">
+      <c r="B2" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C2" s="11" t="inlineStr">
+      <c r="C2" s="12" t="inlineStr">
         <is>
           <t>Android</t>
         </is>
       </c>
-      <c r="D2" s="11" t="inlineStr">
+      <c r="D2" s="12" t="inlineStr">
         <is>
           <t>Text fields with sensitive data</t>
         </is>
       </c>
-      <c r="E2" s="11" t="inlineStr">
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>Set Text suggestions to .none 
  android:inputType="textNoSuggestions"</t>
         </is>
       </c>
-      <c r="F2" s="11" t="inlineStr"/>
-      <c r="G2" s="12">
-        <f>IFERROR(A2+E2+"x",TODAY())</f>
+      <c r="F2" s="12" t="inlineStr"/>
+      <c r="G2" s="13">
+        <f>IFERROR(B2+F22+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H2" s="11" t="inlineStr">
+      <c r="H2" s="12" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I2" s="13" t="inlineStr">
+      <c r="I2" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="inlineStr">
+      <c r="A3" s="12" t="inlineStr">
         <is>
           <t>AND.2</t>
         </is>
       </c>
-      <c r="B3" s="11" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C3" s="11" t="inlineStr">
+      <c r="C3" s="12" t="inlineStr">
         <is>
           <t>Android</t>
         </is>
       </c>
-      <c r="D3" s="11" t="inlineStr">
+      <c r="D3" s="12" t="inlineStr">
         <is>
           <t>Android App, when app shows sensitive data like medical, banking, etc. 
  Easy to implement, but it should not be implemented over usability in some apps like messenger</t>
         </is>
       </c>
-      <c r="E3" s="11" t="inlineStr">
+      <c r="E3" s="12" t="inlineStr">
         <is>
           <t>Android Screenshot / screen recording preventing, 
  Android offers a screenshot feature that can be used by the user or by the system for recent apps. 
  Due to that reason screenshots should be disable for sensitive data</t>
         </is>
       </c>
-      <c r="F3" s="11" t="inlineStr"/>
-      <c r="G3" s="12">
-        <f>IFERROR(A3+E3+"x",TODAY())</f>
+      <c r="F3" s="12" t="inlineStr"/>
+      <c r="G3" s="13">
+        <f>IFERROR(B3+F33+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H3" s="11" t="inlineStr">
+      <c r="H3" s="12" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I3" s="13" t="inlineStr">
+      <c r="I3" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="inlineStr">
+      <c r="A4" s="12" t="inlineStr">
         <is>
           <t>AND.3</t>
         </is>
       </c>
-      <c r="B4" s="11" t="inlineStr">
+      <c r="B4" s="12" t="inlineStr">
         <is>
           <t>TODO</t>
         </is>
       </c>
-      <c r="C4" s="11" t="inlineStr">
+      <c r="C4" s="12" t="inlineStr">
         <is>
           <t>Android</t>
         </is>
       </c>
-      <c r="D4" s="11" t="inlineStr">
+      <c r="D4" s="12" t="inlineStr">
         <is>
           <t>Fields with sensitive data that should not be copied</t>
         </is>
       </c>
-      <c r="E4" s="11" t="inlineStr">
+      <c r="E4" s="12" t="inlineStr">
         <is>
           <t>Secure fields with sensitive data from coping them by other apps and User</t>
         </is>
       </c>
-      <c r="F4" s="11" t="inlineStr"/>
-      <c r="G4" s="12">
-        <f>IFERROR(A4+E4+"x",TODAY())</f>
+      <c r="F4" s="12" t="inlineStr"/>
+      <c r="G4" s="13">
+        <f>IFERROR(B4+F44+"x",TODAY())</f>
         <v/>
       </c>
-      <c r="H4" s="11" t="inlineStr">
+      <c r="H4" s="12" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I4" s="13" t="inlineStr">
+      <c r="I4" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
@@ -2844,7 +2847,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2901,13 +2904,13 @@
         </is>
       </c>
       <c r="B2" s="4" t="n"/>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>- first name
-- last name
-- phone number
-- blood type
-- list of diseases</t>
+      <c r="C2" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - first name
+  - last name
+  - phone number
+  - blood type
+  - list of diseases</t>
         </is>
       </c>
       <c r="D2" s="4" t="n"/>
@@ -2941,11 +2944,11 @@
         </is>
       </c>
       <c r="B3" s="4" t="n"/>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>- first name
-- last name
-- phone number</t>
+      <c r="C3" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - first name
+  - last name
+  - phone number</t>
         </is>
       </c>
       <c r="D3" s="4" t="n"/>
@@ -2979,13 +2982,13 @@
         </is>
       </c>
       <c r="B4" s="4" t="n"/>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>- first name
-- last name
-- phone number
-- blood type
-- list of diseases</t>
+      <c r="C4" s="10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - first name
+  - last name
+  - phone number
+  - blood type
+  - list of diseases</t>
         </is>
       </c>
       <c r="D4" s="4" t="n"/>

</xml_diff>

<commit_message>
Create external libraries linking requirement
</commit_message>
<xml_diff>
--- a/mobile_security_checklist.xlsx
+++ b/mobile_security_checklist.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Shared" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="iOS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Android" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Data model" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shared" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iOS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Android" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data model" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$38</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iOS'!$C$1:$C$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iOS'!$C$1:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Android'!$C$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
@@ -439,7 +439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
@@ -571,10 +571,10 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B6" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B7" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B8" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -582,12 +582,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1754,7 +1754,7 @@
     <row r="28">
       <c r="A28" s="12" t="inlineStr">
         <is>
-          <t>SW.1</t>
+          <t>SE.9</t>
         </is>
       </c>
       <c r="B28" s="12" t="inlineStr">
@@ -1764,17 +1764,17 @@
       </c>
       <c r="C28" s="12" t="inlineStr">
         <is>
-          <t>WebView</t>
+          <t>Extra</t>
         </is>
       </c>
       <c r="D28" s="12" t="inlineStr">
         <is>
-          <t>App is using webview</t>
+          <t>App receives data from user input</t>
         </is>
       </c>
       <c r="E28" s="12" t="inlineStr">
         <is>
-          <t>JavaScript is disabled in WebViews unless explicitly required</t>
+          <t>Input data should be properly validated to process it safely</t>
         </is>
       </c>
       <c r="F28" s="12" t="inlineStr"/>
@@ -1796,7 +1796,7 @@
     <row r="29">
       <c r="A29" s="12" t="inlineStr">
         <is>
-          <t>SU.1</t>
+          <t>SW.1</t>
         </is>
       </c>
       <c r="B29" s="12" t="inlineStr">
@@ -1806,17 +1806,17 @@
       </c>
       <c r="C29" s="12" t="inlineStr">
         <is>
-          <t>Upload</t>
+          <t>WebView</t>
         </is>
       </c>
       <c r="D29" s="12" t="inlineStr">
         <is>
-          <t>App has file upload</t>
+          <t>App is using webview</t>
         </is>
       </c>
       <c r="E29" s="12" t="inlineStr">
         <is>
-          <t>Limit maximum number of files that can be uploaded at once</t>
+          <t>JavaScript is disabled in WebViews unless explicitly required</t>
         </is>
       </c>
       <c r="F29" s="12" t="inlineStr"/>
@@ -1838,7 +1838,7 @@
     <row r="30">
       <c r="A30" s="12" t="inlineStr">
         <is>
-          <t>SG.1</t>
+          <t>SU.1</t>
         </is>
       </c>
       <c r="B30" s="12" t="inlineStr">
@@ -1848,17 +1848,17 @@
       </c>
       <c r="C30" s="12" t="inlineStr">
         <is>
-          <t>GDPR</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="D30" s="12" t="inlineStr">
         <is>
-          <t>Persising user personal information (name, phone, email, ...) on the device</t>
+          <t>App has file upload</t>
         </is>
       </c>
       <c r="E30" s="12" t="inlineStr">
         <is>
-          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
+          <t>Limit maximum number of files that can be uploaded at once</t>
         </is>
       </c>
       <c r="F30" s="12" t="inlineStr"/>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="H30" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I30" s="14" t="inlineStr">
@@ -1880,7 +1880,7 @@
     <row r="31">
       <c r="A31" s="12" t="inlineStr">
         <is>
-          <t>SG.2</t>
+          <t>SG.1</t>
         </is>
       </c>
       <c r="B31" s="12" t="inlineStr">
@@ -1895,12 +1895,12 @@
       </c>
       <c r="D31" s="12" t="inlineStr">
         <is>
-          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
+          <t>Persising user personal information (name, phone, email, ...) on the device</t>
         </is>
       </c>
       <c r="E31" s="12" t="inlineStr">
         <is>
-          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
+          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
         </is>
       </c>
       <c r="F31" s="12" t="inlineStr"/>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="H31" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I31" s="14" t="inlineStr">
@@ -1922,7 +1922,7 @@
     <row r="32">
       <c r="A32" s="12" t="inlineStr">
         <is>
-          <t>SG.3</t>
+          <t>SG.2</t>
         </is>
       </c>
       <c r="B32" s="12" t="inlineStr">
@@ -1937,12 +1937,12 @@
       </c>
       <c r="D32" s="12" t="inlineStr">
         <is>
-          <t>Sending personal data outside of the application</t>
+          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
         </is>
       </c>
       <c r="E32" s="12" t="inlineStr">
         <is>
-          <t>All requests must be authenticated</t>
+          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
         </is>
       </c>
       <c r="F32" s="12" t="inlineStr"/>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="H32" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I32" s="14" t="inlineStr">
@@ -1964,7 +1964,7 @@
     <row r="33">
       <c r="A33" s="12" t="inlineStr">
         <is>
-          <t>SG.4</t>
+          <t>SG.3</t>
         </is>
       </c>
       <c r="B33" s="12" t="inlineStr">
@@ -1979,12 +1979,12 @@
       </c>
       <c r="D33" s="12" t="inlineStr">
         <is>
-          <t>Transferin personal data through REST API</t>
+          <t>Sending personal data outside of the application</t>
         </is>
       </c>
       <c r="E33" s="12" t="inlineStr">
         <is>
-          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
+          <t>All requests must be authenticated</t>
         </is>
       </c>
       <c r="F33" s="12" t="inlineStr"/>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="H33" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I33" s="14" t="inlineStr">
@@ -2006,7 +2006,7 @@
     <row r="34">
       <c r="A34" s="12" t="inlineStr">
         <is>
-          <t>SG.5</t>
+          <t>SG.4</t>
         </is>
       </c>
       <c r="B34" s="12" t="inlineStr">
@@ -2021,12 +2021,12 @@
       </c>
       <c r="D34" s="12" t="inlineStr">
         <is>
-          <t>Displaying privacy policy screen during registration process</t>
+          <t>Transferin personal data through REST API</t>
         </is>
       </c>
       <c r="E34" s="12" t="inlineStr">
         <is>
-          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
+          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
         </is>
       </c>
       <c r="F34" s="12" t="inlineStr"/>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="H34" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I34" s="14" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
         <is>
-          <t>SG.6</t>
+          <t>SG.5</t>
         </is>
       </c>
       <c r="B35" s="12" t="inlineStr">
@@ -2063,12 +2063,12 @@
       </c>
       <c r="D35" s="12" t="inlineStr">
         <is>
-          <t>Using non-production environments</t>
+          <t>Displaying privacy policy screen during registration process</t>
         </is>
       </c>
       <c r="E35" s="12" t="inlineStr">
         <is>
-          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
+          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
         </is>
       </c>
       <c r="F35" s="12" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="H35" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I35" s="14" t="inlineStr">
@@ -2090,7 +2090,7 @@
     <row r="36">
       <c r="A36" s="12" t="inlineStr">
         <is>
-          <t>SEM.1</t>
+          <t>SG.6</t>
         </is>
       </c>
       <c r="B36" s="12" t="inlineStr">
@@ -2100,17 +2100,17 @@
       </c>
       <c r="C36" s="12" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>GDPR</t>
         </is>
       </c>
       <c r="D36" s="12" t="inlineStr">
         <is>
-          <t>Application has input for user email address</t>
+          <t>Using non-production environments</t>
         </is>
       </c>
       <c r="E36" s="12" t="inlineStr">
         <is>
-          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
+          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
         </is>
       </c>
       <c r="F36" s="12" t="inlineStr"/>
@@ -2132,7 +2132,7 @@
     <row r="37">
       <c r="A37" s="12" t="inlineStr">
         <is>
-          <t>SV.1</t>
+          <t>SEM.1</t>
         </is>
       </c>
       <c r="B37" s="12" t="inlineStr">
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C37" s="12" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="D37" s="12" t="inlineStr">
         <is>
-          <t>User can play video in the application</t>
+          <t>Application has input for user email address</t>
         </is>
       </c>
       <c r="E37" s="12" t="inlineStr">
         <is>
-          <t>Video data must be received through HTTPS protocol</t>
+          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
         </is>
       </c>
       <c r="F37" s="12" t="inlineStr"/>
@@ -2174,7 +2174,7 @@
     <row r="38">
       <c r="A38" s="12" t="inlineStr">
         <is>
-          <t>SL.1</t>
+          <t>SV.1</t>
         </is>
       </c>
       <c r="B38" s="12" t="inlineStr">
@@ -2184,17 +2184,17 @@
       </c>
       <c r="C38" s="12" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D38" s="12" t="inlineStr">
         <is>
-          <t>App is using location services</t>
+          <t>User can play video in the application</t>
         </is>
       </c>
       <c r="E38" s="12" t="inlineStr">
         <is>
-          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+          <t>Video data must be received through HTTPS protocol</t>
         </is>
       </c>
       <c r="F38" s="12" t="inlineStr"/>
@@ -2204,17 +2204,59 @@
       </c>
       <c r="H38" s="12" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I38" s="14" t="inlineStr">
+        <is>
+          <t>Handbook</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="12" t="inlineStr">
+        <is>
+          <t>SL.1</t>
+        </is>
+      </c>
+      <c r="B39" s="12" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="C39" s="12" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D39" s="12" t="inlineStr">
+        <is>
+          <t>App is using location services</t>
+        </is>
+      </c>
+      <c r="E39" s="12" t="inlineStr">
+        <is>
+          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+        </is>
+      </c>
+      <c r="F39" s="12" t="inlineStr"/>
+      <c r="G39" s="13">
+        <f>IFERROR(B39+F3939+"x",TODAY())</f>
+        <v/>
+      </c>
+      <c r="H39" s="12" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I38" s="14" t="inlineStr">
+      <c r="I39" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C38"/>
+  <autoFilter ref="C1:C39"/>
   <conditionalFormatting sqref="A2:I980">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$B2="TODO"</formula>
@@ -2230,63 +2272,64 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38 B39" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"TODO,DONE,Won't fix,Not applicable"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"Critical,High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="I11" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I13" r:id="rId12"/>
-    <hyperlink ref="I14" r:id="rId13"/>
-    <hyperlink ref="I15" r:id="rId14"/>
-    <hyperlink ref="I16" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
-    <hyperlink ref="I18" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I20" r:id="rId19"/>
-    <hyperlink ref="I21" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
-    <hyperlink ref="I23" r:id="rId22"/>
-    <hyperlink ref="I24" r:id="rId23"/>
-    <hyperlink ref="I25" r:id="rId24"/>
-    <hyperlink ref="I26" r:id="rId25"/>
-    <hyperlink ref="I27" r:id="rId26"/>
-    <hyperlink ref="I28" r:id="rId27"/>
-    <hyperlink ref="I29" r:id="rId28"/>
-    <hyperlink ref="I30" r:id="rId29"/>
-    <hyperlink ref="I31" r:id="rId30"/>
-    <hyperlink ref="I32" r:id="rId31"/>
-    <hyperlink ref="I33" r:id="rId32"/>
-    <hyperlink ref="I34" r:id="rId33"/>
-    <hyperlink ref="I35" r:id="rId34"/>
-    <hyperlink ref="I36" r:id="rId35"/>
-    <hyperlink ref="I37" r:id="rId36"/>
-    <hyperlink ref="I38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I17" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I27" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I28" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I29" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I30" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I31" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I32" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I39" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2566,8 +2609,50 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>iOS.6</t>
+        </is>
+      </c>
+      <c r="B7" s="12" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="C7" s="12" t="inlineStr">
+        <is>
+          <t>iOS</t>
+        </is>
+      </c>
+      <c r="D7" s="12" t="inlineStr">
+        <is>
+          <t>Using external libraries</t>
+        </is>
+      </c>
+      <c r="E7" s="12" t="inlineStr">
+        <is>
+          <t>External libraries should be linked staticly</t>
+        </is>
+      </c>
+      <c r="F7" s="12" t="inlineStr"/>
+      <c r="G7" s="13">
+        <f>IFERROR(B7+F77+"x",TODAY())</f>
+        <v/>
+      </c>
+      <c r="H7" s="12" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I7" s="14" t="inlineStr">
+        <is>
+          <t>Handbook</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C6"/>
+  <autoFilter ref="C1:C7"/>
   <conditionalFormatting sqref="A2:I980">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$B2="TODO"</formula>
@@ -2583,26 +2668,27 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation sqref="B2 B3 B4 B5 B6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B2 B3 B4 B5 B6 B7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"TODO,DONE,Won't fix,Not applicable"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2 H3 H4 H5 H6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="H2 H3 H4 H5 H6 H7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"Critical,High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2829,9 +2915,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
run script to generate xlsx
</commit_message>
<xml_diff>
--- a/mobile_security_checklist.xlsx
+++ b/mobile_security_checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shared" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iOS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Android" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data model" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Shared" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="iOS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Android" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Data model" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$39</definedName>
@@ -439,7 +439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
@@ -571,10 +571,10 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B6" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B7" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B8" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B9" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -582,7 +582,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2280,51 +2280,51 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I10" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I11" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I12" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I13" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I14" r:id="rId13"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I15" r:id="rId14"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I16" r:id="rId15"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I17" r:id="rId16"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I18" r:id="rId17"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I19" r:id="rId18"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I20" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I21" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I22" r:id="rId21"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I23" r:id="rId22"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I24" r:id="rId23"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I25" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I26" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I27" r:id="rId26"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I28" r:id="rId27"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I29" r:id="rId28"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I30" r:id="rId29"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I31" r:id="rId30"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I32" r:id="rId31"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I33" r:id="rId32"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I34" r:id="rId33"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I35" r:id="rId34"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I36" r:id="rId35"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I37" r:id="rId36"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I38" r:id="rId37"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I39" r:id="rId38"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
+    <hyperlink ref="I11" r:id="rId10"/>
+    <hyperlink ref="I12" r:id="rId11"/>
+    <hyperlink ref="I13" r:id="rId12"/>
+    <hyperlink ref="I14" r:id="rId13"/>
+    <hyperlink ref="I15" r:id="rId14"/>
+    <hyperlink ref="I16" r:id="rId15"/>
+    <hyperlink ref="I17" r:id="rId16"/>
+    <hyperlink ref="I18" r:id="rId17"/>
+    <hyperlink ref="I19" r:id="rId18"/>
+    <hyperlink ref="I20" r:id="rId19"/>
+    <hyperlink ref="I21" r:id="rId20"/>
+    <hyperlink ref="I22" r:id="rId21"/>
+    <hyperlink ref="I23" r:id="rId22"/>
+    <hyperlink ref="I24" r:id="rId23"/>
+    <hyperlink ref="I25" r:id="rId24"/>
+    <hyperlink ref="I26" r:id="rId25"/>
+    <hyperlink ref="I27" r:id="rId26"/>
+    <hyperlink ref="I28" r:id="rId27"/>
+    <hyperlink ref="I29" r:id="rId28"/>
+    <hyperlink ref="I30" r:id="rId29"/>
+    <hyperlink ref="I31" r:id="rId30"/>
+    <hyperlink ref="I32" r:id="rId31"/>
+    <hyperlink ref="I33" r:id="rId32"/>
+    <hyperlink ref="I34" r:id="rId33"/>
+    <hyperlink ref="I35" r:id="rId34"/>
+    <hyperlink ref="I36" r:id="rId35"/>
+    <hyperlink ref="I37" r:id="rId36"/>
+    <hyperlink ref="I38" r:id="rId37"/>
+    <hyperlink ref="I39" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2676,19 +2676,19 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" r:id="rId6"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2915,9 +2915,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add deep links requirement
</commit_message>
<xml_diff>
--- a/mobile_security_checklist.xlsx
+++ b/mobile_security_checklist.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Shared" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="iOS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Android" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Data model" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shared" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iOS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Android" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data model" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iOS'!$C$1:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iOS'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Android'!$C$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
@@ -439,7 +439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
@@ -571,10 +571,10 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B6" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B7" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B8" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -582,12 +582,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1349,12 +1349,12 @@
       </c>
       <c r="D18" s="12" t="inlineStr">
         <is>
-          <t>User enter sensitive data or password into inputs</t>
+          <t>Application contains deep / universal links</t>
         </is>
       </c>
       <c r="E18" s="12" t="inlineStr">
         <is>
-          <t>Disable additional hardware keyboard connected to device, user can only use fabric one</t>
+          <t>App verifies content of deep links according to best practices</t>
         </is>
       </c>
       <c r="F18" s="12" t="inlineStr"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="H18" s="12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I18" s="14" t="inlineStr">
@@ -1796,7 +1796,7 @@
     <row r="29">
       <c r="A29" s="12" t="inlineStr">
         <is>
-          <t>SW.1</t>
+          <t>SE.10</t>
         </is>
       </c>
       <c r="B29" s="12" t="inlineStr">
@@ -1806,17 +1806,17 @@
       </c>
       <c r="C29" s="12" t="inlineStr">
         <is>
-          <t>WebView</t>
+          <t>Extra</t>
         </is>
       </c>
       <c r="D29" s="12" t="inlineStr">
         <is>
-          <t>App is using webview</t>
+          <t>App properly configures auto-correction</t>
         </is>
       </c>
       <c r="E29" s="12" t="inlineStr">
         <is>
-          <t>JavaScript is disabled in WebViews unless explicitly required</t>
+          <t>Auto-correction should be disabled for sensitive input</t>
         </is>
       </c>
       <c r="F29" s="12" t="inlineStr"/>
@@ -1838,7 +1838,7 @@
     <row r="30">
       <c r="A30" s="12" t="inlineStr">
         <is>
-          <t>SU.1</t>
+          <t>SW.1</t>
         </is>
       </c>
       <c r="B30" s="12" t="inlineStr">
@@ -1848,17 +1848,17 @@
       </c>
       <c r="C30" s="12" t="inlineStr">
         <is>
-          <t>Upload</t>
+          <t>WebView</t>
         </is>
       </c>
       <c r="D30" s="12" t="inlineStr">
         <is>
-          <t>App has file upload</t>
+          <t>App is using webview</t>
         </is>
       </c>
       <c r="E30" s="12" t="inlineStr">
         <is>
-          <t>Limit maximum number of files that can be uploaded at once</t>
+          <t>JavaScript is disabled in WebViews unless explicitly required</t>
         </is>
       </c>
       <c r="F30" s="12" t="inlineStr"/>
@@ -1880,7 +1880,7 @@
     <row r="31">
       <c r="A31" s="12" t="inlineStr">
         <is>
-          <t>SG.1</t>
+          <t>SU.1</t>
         </is>
       </c>
       <c r="B31" s="12" t="inlineStr">
@@ -1890,17 +1890,17 @@
       </c>
       <c r="C31" s="12" t="inlineStr">
         <is>
-          <t>GDPR</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="D31" s="12" t="inlineStr">
         <is>
-          <t>Persising user personal information (name, phone, email, ...) on the device</t>
+          <t>App has file upload</t>
         </is>
       </c>
       <c r="E31" s="12" t="inlineStr">
         <is>
-          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
+          <t>Limit maximum number of files that can be uploaded at once</t>
         </is>
       </c>
       <c r="F31" s="12" t="inlineStr"/>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="H31" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I31" s="14" t="inlineStr">
@@ -1922,7 +1922,7 @@
     <row r="32">
       <c r="A32" s="12" t="inlineStr">
         <is>
-          <t>SG.2</t>
+          <t>SG.1</t>
         </is>
       </c>
       <c r="B32" s="12" t="inlineStr">
@@ -1937,12 +1937,12 @@
       </c>
       <c r="D32" s="12" t="inlineStr">
         <is>
-          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
+          <t>Persising user personal information (name, phone, email, ...) on the device</t>
         </is>
       </c>
       <c r="E32" s="12" t="inlineStr">
         <is>
-          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
+          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
         </is>
       </c>
       <c r="F32" s="12" t="inlineStr"/>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="H32" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I32" s="14" t="inlineStr">
@@ -1964,7 +1964,7 @@
     <row r="33">
       <c r="A33" s="12" t="inlineStr">
         <is>
-          <t>SG.3</t>
+          <t>SG.2</t>
         </is>
       </c>
       <c r="B33" s="12" t="inlineStr">
@@ -1979,12 +1979,12 @@
       </c>
       <c r="D33" s="12" t="inlineStr">
         <is>
-          <t>Sending personal data outside of the application</t>
+          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
         </is>
       </c>
       <c r="E33" s="12" t="inlineStr">
         <is>
-          <t>All requests must be authenticated</t>
+          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
         </is>
       </c>
       <c r="F33" s="12" t="inlineStr"/>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="H33" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I33" s="14" t="inlineStr">
@@ -2006,7 +2006,7 @@
     <row r="34">
       <c r="A34" s="12" t="inlineStr">
         <is>
-          <t>SG.4</t>
+          <t>SG.3</t>
         </is>
       </c>
       <c r="B34" s="12" t="inlineStr">
@@ -2021,12 +2021,12 @@
       </c>
       <c r="D34" s="12" t="inlineStr">
         <is>
-          <t>Transferin personal data through REST API</t>
+          <t>Sending personal data outside of the application</t>
         </is>
       </c>
       <c r="E34" s="12" t="inlineStr">
         <is>
-          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
+          <t>All requests must be authenticated</t>
         </is>
       </c>
       <c r="F34" s="12" t="inlineStr"/>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="H34" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I34" s="14" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
         <is>
-          <t>SG.5</t>
+          <t>SG.4</t>
         </is>
       </c>
       <c r="B35" s="12" t="inlineStr">
@@ -2063,12 +2063,12 @@
       </c>
       <c r="D35" s="12" t="inlineStr">
         <is>
-          <t>Displaying privacy policy screen during registration process</t>
+          <t>Transferin personal data through REST API</t>
         </is>
       </c>
       <c r="E35" s="12" t="inlineStr">
         <is>
-          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
+          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
         </is>
       </c>
       <c r="F35" s="12" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="H35" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I35" s="14" t="inlineStr">
@@ -2090,7 +2090,7 @@
     <row r="36">
       <c r="A36" s="12" t="inlineStr">
         <is>
-          <t>SG.6</t>
+          <t>SG.5</t>
         </is>
       </c>
       <c r="B36" s="12" t="inlineStr">
@@ -2105,12 +2105,12 @@
       </c>
       <c r="D36" s="12" t="inlineStr">
         <is>
-          <t>Using non-production environments</t>
+          <t>Displaying privacy policy screen during registration process</t>
         </is>
       </c>
       <c r="E36" s="12" t="inlineStr">
         <is>
-          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
+          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
         </is>
       </c>
       <c r="F36" s="12" t="inlineStr"/>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="H36" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I36" s="14" t="inlineStr">
@@ -2132,7 +2132,7 @@
     <row r="37">
       <c r="A37" s="12" t="inlineStr">
         <is>
-          <t>SEM.1</t>
+          <t>SG.6</t>
         </is>
       </c>
       <c r="B37" s="12" t="inlineStr">
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C37" s="12" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>GDPR</t>
         </is>
       </c>
       <c r="D37" s="12" t="inlineStr">
         <is>
-          <t>Application has input for user email address</t>
+          <t>Using non-production environments</t>
         </is>
       </c>
       <c r="E37" s="12" t="inlineStr">
         <is>
-          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
+          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
         </is>
       </c>
       <c r="F37" s="12" t="inlineStr"/>
@@ -2174,7 +2174,7 @@
     <row r="38">
       <c r="A38" s="12" t="inlineStr">
         <is>
-          <t>SV.1</t>
+          <t>SEM.1</t>
         </is>
       </c>
       <c r="B38" s="12" t="inlineStr">
@@ -2184,17 +2184,17 @@
       </c>
       <c r="C38" s="12" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="D38" s="12" t="inlineStr">
         <is>
-          <t>User can play video in the application</t>
+          <t>Application has input for user email address</t>
         </is>
       </c>
       <c r="E38" s="12" t="inlineStr">
         <is>
-          <t>Video data must be received through HTTPS protocol</t>
+          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
         </is>
       </c>
       <c r="F38" s="12" t="inlineStr"/>
@@ -2216,7 +2216,7 @@
     <row r="39">
       <c r="A39" s="12" t="inlineStr">
         <is>
-          <t>SL.1</t>
+          <t>SV.1</t>
         </is>
       </c>
       <c r="B39" s="12" t="inlineStr">
@@ -2226,17 +2226,17 @@
       </c>
       <c r="C39" s="12" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D39" s="12" t="inlineStr">
         <is>
-          <t>App is using location services</t>
+          <t>User can play video in the application</t>
         </is>
       </c>
       <c r="E39" s="12" t="inlineStr">
         <is>
-          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+          <t>Video data must be received through HTTPS protocol</t>
         </is>
       </c>
       <c r="F39" s="12" t="inlineStr"/>
@@ -2246,17 +2246,59 @@
       </c>
       <c r="H39" s="12" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I39" s="14" t="inlineStr">
+        <is>
+          <t>Handbook</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="12" t="inlineStr">
+        <is>
+          <t>SL.1</t>
+        </is>
+      </c>
+      <c r="B40" s="12" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="C40" s="12" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D40" s="12" t="inlineStr">
+        <is>
+          <t>App is using location services</t>
+        </is>
+      </c>
+      <c r="E40" s="12" t="inlineStr">
+        <is>
+          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+        </is>
+      </c>
+      <c r="F40" s="12" t="inlineStr"/>
+      <c r="G40" s="13">
+        <f>IFERROR(B40+F4040+"x",TODAY())</f>
+        <v/>
+      </c>
+      <c r="H40" s="12" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I39" s="14" t="inlineStr">
+      <c r="I40" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C39"/>
+  <autoFilter ref="C1:C40"/>
   <conditionalFormatting sqref="A2:I980">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$B2="TODO"</formula>
@@ -2272,64 +2314,65 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38 B39" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38 B39 B40" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"TODO,DONE,Won't fix,Not applicable"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"Critical,High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="I11" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I13" r:id="rId12"/>
-    <hyperlink ref="I14" r:id="rId13"/>
-    <hyperlink ref="I15" r:id="rId14"/>
-    <hyperlink ref="I16" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
-    <hyperlink ref="I18" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I20" r:id="rId19"/>
-    <hyperlink ref="I21" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
-    <hyperlink ref="I23" r:id="rId22"/>
-    <hyperlink ref="I24" r:id="rId23"/>
-    <hyperlink ref="I25" r:id="rId24"/>
-    <hyperlink ref="I26" r:id="rId25"/>
-    <hyperlink ref="I27" r:id="rId26"/>
-    <hyperlink ref="I28" r:id="rId27"/>
-    <hyperlink ref="I29" r:id="rId28"/>
-    <hyperlink ref="I30" r:id="rId29"/>
-    <hyperlink ref="I31" r:id="rId30"/>
-    <hyperlink ref="I32" r:id="rId31"/>
-    <hyperlink ref="I33" r:id="rId32"/>
-    <hyperlink ref="I34" r:id="rId33"/>
-    <hyperlink ref="I35" r:id="rId34"/>
-    <hyperlink ref="I36" r:id="rId35"/>
-    <hyperlink ref="I37" r:id="rId36"/>
-    <hyperlink ref="I38" r:id="rId37"/>
-    <hyperlink ref="I39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I17" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I18" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I19" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I20" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I21" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I22" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I23" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I24" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I25" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I26" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I27" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I28" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I29" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I30" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I31" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I32" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I40" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2414,12 +2457,13 @@
       </c>
       <c r="D2" s="12" t="inlineStr">
         <is>
-          <t>Using UITextField with sensitive data</t>
+          <t>Using NSURLSession</t>
         </is>
       </c>
       <c r="E2" s="12" t="inlineStr">
         <is>
-          <t>Set autocorrectionType to .none in Sensitive UITextFields</t>
+          <t>By default NSURLSession stores data, such as HTTP requests and responses in the Cache.db database. 
+ It should be disabled in URLSession with setting .ephemeral type instead of default one</t>
         </is>
       </c>
       <c r="F2" s="12" t="inlineStr"/>
@@ -2429,7 +2473,7 @@
       </c>
       <c r="H2" s="12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I2" s="14" t="inlineStr">
@@ -2456,13 +2500,13 @@
       </c>
       <c r="D3" s="12" t="inlineStr">
         <is>
-          <t>Using NSURLSession</t>
+          <t>Certificate Pinning implemetation using TrustKit</t>
         </is>
       </c>
       <c r="E3" s="12" t="inlineStr">
         <is>
-          <t>By default NSURLSession stores data, such as HTTP requests and responses in the Cache.db database. 
- It should be disabled in URLSession with setting .ephemeral type instead of default one</t>
+          <t>Set kTSKDisableDefaultReportUri to true 
+ By default this flag is false, which means it will be sending error reports to tool owner</t>
         </is>
       </c>
       <c r="F3" s="12" t="inlineStr"/>
@@ -2499,13 +2543,13 @@
       </c>
       <c r="D4" s="12" t="inlineStr">
         <is>
-          <t>Certificate Pinning implemetation using TrustKit</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="E4" s="12" t="inlineStr">
         <is>
-          <t>Set kTSKDisableDefaultReportUri to true 
- By default this flag is false, which means it will be sending error reports to tool owner</t>
+          <t>Verify if not needed files are not included in the bundle. 
+ Exclude them if needed using EXCLUDED_SOURCE_FILE_NAMES</t>
         </is>
       </c>
       <c r="F4" s="12" t="inlineStr"/>
@@ -2515,7 +2559,7 @@
       </c>
       <c r="H4" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I4" s="14" t="inlineStr">
@@ -2542,13 +2586,12 @@
       </c>
       <c r="D5" s="12" t="inlineStr">
         <is>
-          <t>Default</t>
+          <t>User enter sensitive data or password into inputs</t>
         </is>
       </c>
       <c r="E5" s="12" t="inlineStr">
         <is>
-          <t>Verify if not needed files are not included in the bundle. 
- Exclude them if needed using EXCLUDED_SOURCE_FILE_NAMES</t>
+          <t>Verify that the app prevents usage of custom third-party keyboards whenever sensitive data is entered</t>
         </is>
       </c>
       <c r="F5" s="12" t="inlineStr"/>
@@ -2558,7 +2601,7 @@
       </c>
       <c r="H5" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I5" s="14" t="inlineStr">
@@ -2585,12 +2628,12 @@
       </c>
       <c r="D6" s="12" t="inlineStr">
         <is>
-          <t>User enter sensitive data or password into inputs</t>
+          <t>Using external libraries</t>
         </is>
       </c>
       <c r="E6" s="12" t="inlineStr">
         <is>
-          <t>Verify that the app prevents usage of custom third-party keyboards whenever sensitive data is entered</t>
+          <t>External libraries should be linked staticly</t>
         </is>
       </c>
       <c r="F6" s="12" t="inlineStr"/>
@@ -2609,50 +2652,8 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="12" t="inlineStr">
-        <is>
-          <t>iOS.6</t>
-        </is>
-      </c>
-      <c r="B7" s="12" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="C7" s="12" t="inlineStr">
-        <is>
-          <t>iOS</t>
-        </is>
-      </c>
-      <c r="D7" s="12" t="inlineStr">
-        <is>
-          <t>Using external libraries</t>
-        </is>
-      </c>
-      <c r="E7" s="12" t="inlineStr">
-        <is>
-          <t>External libraries should be linked staticly</t>
-        </is>
-      </c>
-      <c r="F7" s="12" t="inlineStr"/>
-      <c r="G7" s="13">
-        <f>IFERROR(B7+F77+"x",TODAY())</f>
-        <v/>
-      </c>
-      <c r="H7" s="12" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="I7" s="14" t="inlineStr">
-        <is>
-          <t>Handbook</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="C1:C7"/>
+  <autoFilter ref="C1:C6"/>
   <conditionalFormatting sqref="A2:I980">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$B2="TODO"</formula>
@@ -2668,27 +2669,26 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation sqref="B2 B3 B4 B5 B6 B7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B2 B3 B4 B5 B6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"TODO,DONE,Won't fix,Not applicable"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2 H3 H4 H5 H6 H7" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="H2 H3 H4 H5 H6" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"Critical,High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2915,9 +2915,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Generate changes to excel
</commit_message>
<xml_diff>
--- a/mobile_security_checklist.xlsx
+++ b/mobile_security_checklist.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shared" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="iOS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Android" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data model" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Getting started" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Shared" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="iOS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Android" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Data model" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iOS'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Android'!$C$1:$C$4</definedName>
   </definedNames>
@@ -439,7 +439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
@@ -571,10 +571,10 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B6" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B7" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B8" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B9" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -582,12 +582,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1418,7 +1418,7 @@
     <row r="20">
       <c r="A20" s="12" t="inlineStr">
         <is>
-          <t>SE.1</t>
+          <t>SD.19</t>
         </is>
       </c>
       <c r="B20" s="12" t="inlineStr">
@@ -1428,17 +1428,17 @@
       </c>
       <c r="C20" s="12" t="inlineStr">
         <is>
-          <t>Extra</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="D20" s="12" t="inlineStr">
         <is>
-          <t>Fintech app or very sensitive application</t>
+          <t>Application contains Development / Debug code</t>
         </is>
       </c>
       <c r="E20" s="12" t="inlineStr">
         <is>
-          <t>To increase security of the application it could be additionally protected with PIN screen</t>
+          <t>This code is not compiled to Production application</t>
         </is>
       </c>
       <c r="F20" s="12" t="inlineStr"/>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="H20" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I20" s="14" t="inlineStr">
@@ -1460,7 +1460,7 @@
     <row r="21">
       <c r="A21" s="12" t="inlineStr">
         <is>
-          <t>SE.2</t>
+          <t>SE.1</t>
         </is>
       </c>
       <c r="B21" s="12" t="inlineStr">
@@ -1475,12 +1475,12 @@
       </c>
       <c r="D21" s="12" t="inlineStr">
         <is>
-          <t>User shouldn't use jailbroken/rooted device</t>
+          <t>Fintech app or very sensitive application</t>
         </is>
       </c>
       <c r="E21" s="12" t="inlineStr">
         <is>
-          <t>The app detects and reacts to the presence of a rooted or jailbroken device either by alerting the user or terminating the app</t>
+          <t>To increase security of the application it could be additionally protected with PIN screen</t>
         </is>
       </c>
       <c r="F21" s="12" t="inlineStr"/>
@@ -1502,7 +1502,7 @@
     <row r="22">
       <c r="A22" s="12" t="inlineStr">
         <is>
-          <t>SE.3</t>
+          <t>SE.2</t>
         </is>
       </c>
       <c r="B22" s="12" t="inlineStr">
@@ -1517,12 +1517,12 @@
       </c>
       <c r="D22" s="12" t="inlineStr">
         <is>
-          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
+          <t>User shouldn't use jailbroken/rooted device</t>
         </is>
       </c>
       <c r="E22" s="12" t="inlineStr">
         <is>
-          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
+          <t>The app detects and reacts to the presence of a rooted or jailbroken device either by alerting the user or terminating the app</t>
         </is>
       </c>
       <c r="F22" s="12" t="inlineStr"/>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="H22" s="12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I22" s="14" t="inlineStr">
@@ -1544,7 +1544,7 @@
     <row r="23">
       <c r="A23" s="12" t="inlineStr">
         <is>
-          <t>SE.4</t>
+          <t>SE.3</t>
         </is>
       </c>
       <c r="B23" s="12" t="inlineStr">
@@ -1559,12 +1559,12 @@
       </c>
       <c r="D23" s="12" t="inlineStr">
         <is>
-          <t>The app catches and handles possible exceptions</t>
+          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
         </is>
       </c>
       <c r="E23" s="12" t="inlineStr">
         <is>
-          <t>Make sure you have added sentry, bugsnag or crashlitics or other to catch all crashes</t>
+          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
         </is>
       </c>
       <c r="F23" s="12" t="inlineStr"/>
@@ -1586,7 +1586,7 @@
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
         <is>
-          <t>SE.5</t>
+          <t>SE.4</t>
         </is>
       </c>
       <c r="B24" s="12" t="inlineStr">
@@ -1601,12 +1601,12 @@
       </c>
       <c r="D24" s="12" t="inlineStr">
         <is>
-          <t>Storing data using hashes</t>
+          <t>The app catches and handles possible exceptions</t>
         </is>
       </c>
       <c r="E24" s="12" t="inlineStr">
         <is>
-          <t>Hashed data should use unique (for every user) salt to increase the complexity of reversing the operation</t>
+          <t>Make sure you have added sentry, bugsnag or crashlitics or other to catch all crashes</t>
         </is>
       </c>
       <c r="F24" s="12" t="inlineStr"/>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="H24" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I24" s="14" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="25">
       <c r="A25" s="12" t="inlineStr">
         <is>
-          <t>SE.6</t>
+          <t>SE.5</t>
         </is>
       </c>
       <c r="B25" s="12" t="inlineStr">
@@ -1643,12 +1643,12 @@
       </c>
       <c r="D25" s="12" t="inlineStr">
         <is>
-          <t>Very sensitive applications like banking apps</t>
+          <t>Storing data using hashes</t>
         </is>
       </c>
       <c r="E25" s="12" t="inlineStr">
         <is>
-          <t>Two factor authentication</t>
+          <t>Hashed data should use unique (for every user) salt to increase the complexity of reversing the operation</t>
         </is>
       </c>
       <c r="F25" s="12" t="inlineStr"/>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="H25" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I25" s="14" t="inlineStr">
@@ -1670,7 +1670,7 @@
     <row r="26">
       <c r="A26" s="12" t="inlineStr">
         <is>
-          <t>SE.7</t>
+          <t>SE.6</t>
         </is>
       </c>
       <c r="B26" s="12" t="inlineStr">
@@ -1685,12 +1685,12 @@
       </c>
       <c r="D26" s="12" t="inlineStr">
         <is>
-          <t>App is recognizing device as trust device</t>
+          <t>Very sensitive applications like banking apps</t>
         </is>
       </c>
       <c r="E26" s="12" t="inlineStr">
         <is>
-          <t>The app implements a 'device binding' functionality using a device fingerprint derived from multiple properties unique to the device</t>
+          <t>Two factor authentication</t>
         </is>
       </c>
       <c r="F26" s="12" t="inlineStr"/>
@@ -1700,7 +1700,7 @@
       </c>
       <c r="H26" s="12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I26" s="14" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="27">
       <c r="A27" s="12" t="inlineStr">
         <is>
-          <t>SE.8</t>
+          <t>SE.7</t>
         </is>
       </c>
       <c r="B27" s="12" t="inlineStr">
@@ -1727,12 +1727,12 @@
       </c>
       <c r="D27" s="12" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>App is recognizing device as trust device</t>
         </is>
       </c>
       <c r="E27" s="12" t="inlineStr">
         <is>
-          <t>Block App after number of login failures</t>
+          <t>The app implements a 'device binding' functionality using a device fingerprint derived from multiple properties unique to the device</t>
         </is>
       </c>
       <c r="F27" s="12" t="inlineStr"/>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="H27" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I27" s="14" t="inlineStr">
@@ -1754,7 +1754,7 @@
     <row r="28">
       <c r="A28" s="12" t="inlineStr">
         <is>
-          <t>SE.9</t>
+          <t>SE.8</t>
         </is>
       </c>
       <c r="B28" s="12" t="inlineStr">
@@ -1769,12 +1769,12 @@
       </c>
       <c r="D28" s="12" t="inlineStr">
         <is>
-          <t>App receives data from user input</t>
+          <t>Login</t>
         </is>
       </c>
       <c r="E28" s="12" t="inlineStr">
         <is>
-          <t>Input data should be properly validated to process it safely</t>
+          <t>Block App after number of login failures</t>
         </is>
       </c>
       <c r="F28" s="12" t="inlineStr"/>
@@ -1796,7 +1796,7 @@
     <row r="29">
       <c r="A29" s="12" t="inlineStr">
         <is>
-          <t>SE.10</t>
+          <t>SE.9</t>
         </is>
       </c>
       <c r="B29" s="12" t="inlineStr">
@@ -1811,12 +1811,12 @@
       </c>
       <c r="D29" s="12" t="inlineStr">
         <is>
-          <t>App properly configures auto-correction</t>
+          <t>App receives data from user input</t>
         </is>
       </c>
       <c r="E29" s="12" t="inlineStr">
         <is>
-          <t>Auto-correction should be disabled for sensitive input</t>
+          <t>Input data should be properly validated to process it safely</t>
         </is>
       </c>
       <c r="F29" s="12" t="inlineStr"/>
@@ -1838,7 +1838,7 @@
     <row r="30">
       <c r="A30" s="12" t="inlineStr">
         <is>
-          <t>SW.1</t>
+          <t>SE.10</t>
         </is>
       </c>
       <c r="B30" s="12" t="inlineStr">
@@ -1848,17 +1848,17 @@
       </c>
       <c r="C30" s="12" t="inlineStr">
         <is>
-          <t>WebView</t>
+          <t>Extra</t>
         </is>
       </c>
       <c r="D30" s="12" t="inlineStr">
         <is>
-          <t>App is using webview</t>
+          <t>App properly configures auto-correction</t>
         </is>
       </c>
       <c r="E30" s="12" t="inlineStr">
         <is>
-          <t>JavaScript is disabled in WebViews unless explicitly required</t>
+          <t>Auto-correction should be disabled for sensitive input</t>
         </is>
       </c>
       <c r="F30" s="12" t="inlineStr"/>
@@ -1880,7 +1880,7 @@
     <row r="31">
       <c r="A31" s="12" t="inlineStr">
         <is>
-          <t>SU.1</t>
+          <t>SW.1</t>
         </is>
       </c>
       <c r="B31" s="12" t="inlineStr">
@@ -1890,17 +1890,17 @@
       </c>
       <c r="C31" s="12" t="inlineStr">
         <is>
-          <t>Upload</t>
+          <t>WebView</t>
         </is>
       </c>
       <c r="D31" s="12" t="inlineStr">
         <is>
-          <t>App has file upload</t>
+          <t>App is using webview</t>
         </is>
       </c>
       <c r="E31" s="12" t="inlineStr">
         <is>
-          <t>Limit maximum number of files that can be uploaded at once</t>
+          <t>JavaScript is disabled in WebViews unless explicitly required</t>
         </is>
       </c>
       <c r="F31" s="12" t="inlineStr"/>
@@ -1922,7 +1922,7 @@
     <row r="32">
       <c r="A32" s="12" t="inlineStr">
         <is>
-          <t>SG.1</t>
+          <t>SU.1</t>
         </is>
       </c>
       <c r="B32" s="12" t="inlineStr">
@@ -1932,17 +1932,17 @@
       </c>
       <c r="C32" s="12" t="inlineStr">
         <is>
-          <t>GDPR</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="D32" s="12" t="inlineStr">
         <is>
-          <t>Persising user personal information (name, phone, email, ...) on the device</t>
+          <t>App has file upload</t>
         </is>
       </c>
       <c r="E32" s="12" t="inlineStr">
         <is>
-          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
+          <t>Limit maximum number of files that can be uploaded at once</t>
         </is>
       </c>
       <c r="F32" s="12" t="inlineStr"/>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="H32" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I32" s="14" t="inlineStr">
@@ -1964,7 +1964,7 @@
     <row r="33">
       <c r="A33" s="12" t="inlineStr">
         <is>
-          <t>SG.2</t>
+          <t>SG.1</t>
         </is>
       </c>
       <c r="B33" s="12" t="inlineStr">
@@ -1979,12 +1979,12 @@
       </c>
       <c r="D33" s="12" t="inlineStr">
         <is>
-          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
+          <t>Persising user personal information (name, phone, email, ...) on the device</t>
         </is>
       </c>
       <c r="E33" s="12" t="inlineStr">
         <is>
-          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
+          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
         </is>
       </c>
       <c r="F33" s="12" t="inlineStr"/>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="H33" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I33" s="14" t="inlineStr">
@@ -2006,7 +2006,7 @@
     <row r="34">
       <c r="A34" s="12" t="inlineStr">
         <is>
-          <t>SG.3</t>
+          <t>SG.2</t>
         </is>
       </c>
       <c r="B34" s="12" t="inlineStr">
@@ -2021,12 +2021,12 @@
       </c>
       <c r="D34" s="12" t="inlineStr">
         <is>
-          <t>Sending personal data outside of the application</t>
+          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
         </is>
       </c>
       <c r="E34" s="12" t="inlineStr">
         <is>
-          <t>All requests must be authenticated</t>
+          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
         </is>
       </c>
       <c r="F34" s="12" t="inlineStr"/>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="H34" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I34" s="14" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
         <is>
-          <t>SG.4</t>
+          <t>SG.3</t>
         </is>
       </c>
       <c r="B35" s="12" t="inlineStr">
@@ -2063,12 +2063,12 @@
       </c>
       <c r="D35" s="12" t="inlineStr">
         <is>
-          <t>Transferin personal data through REST API</t>
+          <t>Sending personal data outside of the application</t>
         </is>
       </c>
       <c r="E35" s="12" t="inlineStr">
         <is>
-          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
+          <t>All requests must be authenticated</t>
         </is>
       </c>
       <c r="F35" s="12" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="H35" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I35" s="14" t="inlineStr">
@@ -2090,7 +2090,7 @@
     <row r="36">
       <c r="A36" s="12" t="inlineStr">
         <is>
-          <t>SG.5</t>
+          <t>SG.4</t>
         </is>
       </c>
       <c r="B36" s="12" t="inlineStr">
@@ -2105,12 +2105,12 @@
       </c>
       <c r="D36" s="12" t="inlineStr">
         <is>
-          <t>Displaying privacy policy screen during registration process</t>
+          <t>Transferin personal data through REST API</t>
         </is>
       </c>
       <c r="E36" s="12" t="inlineStr">
         <is>
-          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
+          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
         </is>
       </c>
       <c r="F36" s="12" t="inlineStr"/>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="H36" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I36" s="14" t="inlineStr">
@@ -2132,7 +2132,7 @@
     <row r="37">
       <c r="A37" s="12" t="inlineStr">
         <is>
-          <t>SG.6</t>
+          <t>SG.5</t>
         </is>
       </c>
       <c r="B37" s="12" t="inlineStr">
@@ -2147,12 +2147,12 @@
       </c>
       <c r="D37" s="12" t="inlineStr">
         <is>
-          <t>Using non-production environments</t>
+          <t>Displaying privacy policy screen during registration process</t>
         </is>
       </c>
       <c r="E37" s="12" t="inlineStr">
         <is>
-          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
+          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
         </is>
       </c>
       <c r="F37" s="12" t="inlineStr"/>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="H37" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I37" s="14" t="inlineStr">
@@ -2174,7 +2174,7 @@
     <row r="38">
       <c r="A38" s="12" t="inlineStr">
         <is>
-          <t>SEM.1</t>
+          <t>SG.6</t>
         </is>
       </c>
       <c r="B38" s="12" t="inlineStr">
@@ -2184,17 +2184,17 @@
       </c>
       <c r="C38" s="12" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>GDPR</t>
         </is>
       </c>
       <c r="D38" s="12" t="inlineStr">
         <is>
-          <t>Application has input for user email address</t>
+          <t>Using non-production environments</t>
         </is>
       </c>
       <c r="E38" s="12" t="inlineStr">
         <is>
-          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
+          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
         </is>
       </c>
       <c r="F38" s="12" t="inlineStr"/>
@@ -2216,7 +2216,7 @@
     <row r="39">
       <c r="A39" s="12" t="inlineStr">
         <is>
-          <t>SV.1</t>
+          <t>SEM.1</t>
         </is>
       </c>
       <c r="B39" s="12" t="inlineStr">
@@ -2226,17 +2226,17 @@
       </c>
       <c r="C39" s="12" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="D39" s="12" t="inlineStr">
         <is>
-          <t>User can play video in the application</t>
+          <t>Application has input for user email address</t>
         </is>
       </c>
       <c r="E39" s="12" t="inlineStr">
         <is>
-          <t>Video data must be received through HTTPS protocol</t>
+          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
         </is>
       </c>
       <c r="F39" s="12" t="inlineStr"/>
@@ -2258,7 +2258,7 @@
     <row r="40">
       <c r="A40" s="12" t="inlineStr">
         <is>
-          <t>SL.1</t>
+          <t>SV.1</t>
         </is>
       </c>
       <c r="B40" s="12" t="inlineStr">
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C40" s="12" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D40" s="12" t="inlineStr">
         <is>
-          <t>App is using location services</t>
+          <t>User can play video in the application</t>
         </is>
       </c>
       <c r="E40" s="12" t="inlineStr">
         <is>
-          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+          <t>Video data must be received through HTTPS protocol</t>
         </is>
       </c>
       <c r="F40" s="12" t="inlineStr"/>
@@ -2288,17 +2288,59 @@
       </c>
       <c r="H40" s="12" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I40" s="14" t="inlineStr">
+        <is>
+          <t>Handbook</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="12" t="inlineStr">
+        <is>
+          <t>SL.1</t>
+        </is>
+      </c>
+      <c r="B41" s="12" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="C41" s="12" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D41" s="12" t="inlineStr">
+        <is>
+          <t>App is using location services</t>
+        </is>
+      </c>
+      <c r="E41" s="12" t="inlineStr">
+        <is>
+          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+        </is>
+      </c>
+      <c r="F41" s="12" t="inlineStr"/>
+      <c r="G41" s="13">
+        <f>IFERROR(B41+F4141+"x",TODAY())</f>
+        <v/>
+      </c>
+      <c r="H41" s="12" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I40" s="14" t="inlineStr">
+      <c r="I41" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C40"/>
+  <autoFilter ref="C1:C41"/>
   <conditionalFormatting sqref="A2:I980">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$B2="TODO"</formula>
@@ -2314,60 +2356,61 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38 B39 B40" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38 B39 B40 B41" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"TODO,DONE,Won't fix,Not applicable"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40 H41" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"Critical,High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I10" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I11" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I12" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I13" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I14" r:id="rId13"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I15" r:id="rId14"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I16" r:id="rId15"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I17" r:id="rId16"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I18" r:id="rId17"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I19" r:id="rId18"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I20" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I21" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I22" r:id="rId21"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I23" r:id="rId22"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I24" r:id="rId23"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I25" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I26" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I27" r:id="rId26"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I28" r:id="rId27"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I29" r:id="rId28"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I30" r:id="rId29"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I31" r:id="rId30"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I32" r:id="rId31"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I33" r:id="rId32"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I34" r:id="rId33"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I35" r:id="rId34"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I36" r:id="rId35"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I37" r:id="rId36"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I38" r:id="rId37"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I39" r:id="rId38"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I40" r:id="rId39"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
+    <hyperlink ref="I11" r:id="rId10"/>
+    <hyperlink ref="I12" r:id="rId11"/>
+    <hyperlink ref="I13" r:id="rId12"/>
+    <hyperlink ref="I14" r:id="rId13"/>
+    <hyperlink ref="I15" r:id="rId14"/>
+    <hyperlink ref="I16" r:id="rId15"/>
+    <hyperlink ref="I17" r:id="rId16"/>
+    <hyperlink ref="I18" r:id="rId17"/>
+    <hyperlink ref="I19" r:id="rId18"/>
+    <hyperlink ref="I20" r:id="rId19"/>
+    <hyperlink ref="I21" r:id="rId20"/>
+    <hyperlink ref="I22" r:id="rId21"/>
+    <hyperlink ref="I23" r:id="rId22"/>
+    <hyperlink ref="I24" r:id="rId23"/>
+    <hyperlink ref="I25" r:id="rId24"/>
+    <hyperlink ref="I26" r:id="rId25"/>
+    <hyperlink ref="I27" r:id="rId26"/>
+    <hyperlink ref="I28" r:id="rId27"/>
+    <hyperlink ref="I29" r:id="rId28"/>
+    <hyperlink ref="I30" r:id="rId29"/>
+    <hyperlink ref="I31" r:id="rId30"/>
+    <hyperlink ref="I32" r:id="rId31"/>
+    <hyperlink ref="I33" r:id="rId32"/>
+    <hyperlink ref="I34" r:id="rId33"/>
+    <hyperlink ref="I35" r:id="rId34"/>
+    <hyperlink ref="I36" r:id="rId35"/>
+    <hyperlink ref="I37" r:id="rId36"/>
+    <hyperlink ref="I38" r:id="rId37"/>
+    <hyperlink ref="I39" r:id="rId38"/>
+    <hyperlink ref="I40" r:id="rId39"/>
+    <hyperlink ref="I41" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2677,18 +2720,18 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId5"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2915,9 +2958,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId3"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Staging protection requirement
</commit_message>
<xml_diff>
--- a/mobile_security_checklist.xlsx
+++ b/mobile_security_checklist.xlsx
@@ -13,7 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data model" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Shared'!$C$1:$C$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iOS'!$C$1:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Android'!$C$1:$C$4</definedName>
   </definedNames>
@@ -587,7 +587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1460,7 +1460,7 @@
     <row r="21">
       <c r="A21" s="12" t="inlineStr">
         <is>
-          <t>SE.1</t>
+          <t>SD.20</t>
         </is>
       </c>
       <c r="B21" s="12" t="inlineStr">
@@ -1470,17 +1470,17 @@
       </c>
       <c r="C21" s="12" t="inlineStr">
         <is>
-          <t>Extra</t>
+          <t>Default</t>
         </is>
       </c>
       <c r="D21" s="12" t="inlineStr">
         <is>
-          <t>Fintech app or very sensitive application</t>
+          <t>Staging offers app functionalities for free</t>
         </is>
       </c>
       <c r="E21" s="12" t="inlineStr">
         <is>
-          <t>To increase security of the application it could be additionally protected with PIN screen</t>
+          <t>It should be protected against random users</t>
         </is>
       </c>
       <c r="F21" s="12" t="inlineStr"/>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="H21" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I21" s="14" t="inlineStr">
@@ -1502,7 +1502,7 @@
     <row r="22">
       <c r="A22" s="12" t="inlineStr">
         <is>
-          <t>SE.2</t>
+          <t>SE.1</t>
         </is>
       </c>
       <c r="B22" s="12" t="inlineStr">
@@ -1517,12 +1517,12 @@
       </c>
       <c r="D22" s="12" t="inlineStr">
         <is>
-          <t>User shouldn't use jailbroken/rooted device</t>
+          <t>Fintech app or very sensitive application</t>
         </is>
       </c>
       <c r="E22" s="12" t="inlineStr">
         <is>
-          <t>The app detects and reacts to the presence of a rooted or jailbroken device either by alerting the user or terminating the app</t>
+          <t>To increase security of the application it could be additionally protected with PIN screen</t>
         </is>
       </c>
       <c r="F22" s="12" t="inlineStr"/>
@@ -1544,7 +1544,7 @@
     <row r="23">
       <c r="A23" s="12" t="inlineStr">
         <is>
-          <t>SE.3</t>
+          <t>SE.2</t>
         </is>
       </c>
       <c r="B23" s="12" t="inlineStr">
@@ -1559,12 +1559,12 @@
       </c>
       <c r="D23" s="12" t="inlineStr">
         <is>
-          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
+          <t>User shouldn't use jailbroken/rooted device</t>
         </is>
       </c>
       <c r="E23" s="12" t="inlineStr">
         <is>
-          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
+          <t>The app detects and reacts to the presence of a rooted or jailbroken device either by alerting the user or terminating the app</t>
         </is>
       </c>
       <c r="F23" s="12" t="inlineStr"/>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="H23" s="12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I23" s="14" t="inlineStr">
@@ -1586,7 +1586,7 @@
     <row r="24">
       <c r="A24" s="12" t="inlineStr">
         <is>
-          <t>SE.4</t>
+          <t>SE.3</t>
         </is>
       </c>
       <c r="B24" s="12" t="inlineStr">
@@ -1601,12 +1601,12 @@
       </c>
       <c r="D24" s="12" t="inlineStr">
         <is>
-          <t>The app catches and handles possible exceptions</t>
+          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
         </is>
       </c>
       <c r="E24" s="12" t="inlineStr">
         <is>
-          <t>Make sure you have added sentry, bugsnag or crashlitics or other to catch all crashes</t>
+          <t>The app informs the user of all sensitive activities with their account. Users are able to view a list of devices, view contextual information (IP address, location, etc.), and to block specific devices</t>
         </is>
       </c>
       <c r="F24" s="12" t="inlineStr"/>
@@ -1628,7 +1628,7 @@
     <row r="25">
       <c r="A25" s="12" t="inlineStr">
         <is>
-          <t>SE.5</t>
+          <t>SE.4</t>
         </is>
       </c>
       <c r="B25" s="12" t="inlineStr">
@@ -1643,12 +1643,12 @@
       </c>
       <c r="D25" s="12" t="inlineStr">
         <is>
-          <t>Storing data using hashes</t>
+          <t>The app catches and handles possible exceptions</t>
         </is>
       </c>
       <c r="E25" s="12" t="inlineStr">
         <is>
-          <t>Hashed data should use unique (for every user) salt to increase the complexity of reversing the operation</t>
+          <t>Make sure you have added sentry, bugsnag or crashlitics or other to catch all crashes</t>
         </is>
       </c>
       <c r="F25" s="12" t="inlineStr"/>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="H25" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I25" s="14" t="inlineStr">
@@ -1670,7 +1670,7 @@
     <row r="26">
       <c r="A26" s="12" t="inlineStr">
         <is>
-          <t>SE.6</t>
+          <t>SE.5</t>
         </is>
       </c>
       <c r="B26" s="12" t="inlineStr">
@@ -1685,12 +1685,12 @@
       </c>
       <c r="D26" s="12" t="inlineStr">
         <is>
-          <t>Very sensitive applications like banking apps</t>
+          <t>Storing data using hashes</t>
         </is>
       </c>
       <c r="E26" s="12" t="inlineStr">
         <is>
-          <t>Two factor authentication</t>
+          <t>Hashed data should use unique (for every user) salt to increase the complexity of reversing the operation</t>
         </is>
       </c>
       <c r="F26" s="12" t="inlineStr"/>
@@ -1700,7 +1700,7 @@
       </c>
       <c r="H26" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I26" s="14" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="27">
       <c r="A27" s="12" t="inlineStr">
         <is>
-          <t>SE.7</t>
+          <t>SE.6</t>
         </is>
       </c>
       <c r="B27" s="12" t="inlineStr">
@@ -1727,12 +1727,12 @@
       </c>
       <c r="D27" s="12" t="inlineStr">
         <is>
-          <t>App is recognizing device as trust device</t>
+          <t>Very sensitive applications like banking apps</t>
         </is>
       </c>
       <c r="E27" s="12" t="inlineStr">
         <is>
-          <t>The app implements a 'device binding' functionality using a device fingerprint derived from multiple properties unique to the device</t>
+          <t>Two factor authentication</t>
         </is>
       </c>
       <c r="F27" s="12" t="inlineStr"/>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="H27" s="12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I27" s="14" t="inlineStr">
@@ -1754,7 +1754,7 @@
     <row r="28">
       <c r="A28" s="12" t="inlineStr">
         <is>
-          <t>SE.8</t>
+          <t>SE.7</t>
         </is>
       </c>
       <c r="B28" s="12" t="inlineStr">
@@ -1769,12 +1769,12 @@
       </c>
       <c r="D28" s="12" t="inlineStr">
         <is>
-          <t>Login</t>
+          <t>App is recognizing device as trust device</t>
         </is>
       </c>
       <c r="E28" s="12" t="inlineStr">
         <is>
-          <t>Block App after number of login failures</t>
+          <t>The app implements a 'device binding' functionality using a device fingerprint derived from multiple properties unique to the device</t>
         </is>
       </c>
       <c r="F28" s="12" t="inlineStr"/>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="H28" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I28" s="14" t="inlineStr">
@@ -1796,7 +1796,7 @@
     <row r="29">
       <c r="A29" s="12" t="inlineStr">
         <is>
-          <t>SE.9</t>
+          <t>SE.8</t>
         </is>
       </c>
       <c r="B29" s="12" t="inlineStr">
@@ -1811,12 +1811,12 @@
       </c>
       <c r="D29" s="12" t="inlineStr">
         <is>
-          <t>App receives data from user input</t>
+          <t>Login</t>
         </is>
       </c>
       <c r="E29" s="12" t="inlineStr">
         <is>
-          <t>Input data should be properly validated to process it safely</t>
+          <t>Block App after number of login failures</t>
         </is>
       </c>
       <c r="F29" s="12" t="inlineStr"/>
@@ -1838,7 +1838,7 @@
     <row r="30">
       <c r="A30" s="12" t="inlineStr">
         <is>
-          <t>SE.10</t>
+          <t>SE.9</t>
         </is>
       </c>
       <c r="B30" s="12" t="inlineStr">
@@ -1853,12 +1853,12 @@
       </c>
       <c r="D30" s="12" t="inlineStr">
         <is>
-          <t>App properly configures auto-correction</t>
+          <t>App receives data from user input</t>
         </is>
       </c>
       <c r="E30" s="12" t="inlineStr">
         <is>
-          <t>Auto-correction should be disabled for sensitive input</t>
+          <t>Input data should be properly validated to process it safely</t>
         </is>
       </c>
       <c r="F30" s="12" t="inlineStr"/>
@@ -1880,7 +1880,7 @@
     <row r="31">
       <c r="A31" s="12" t="inlineStr">
         <is>
-          <t>SW.1</t>
+          <t>SE.10</t>
         </is>
       </c>
       <c r="B31" s="12" t="inlineStr">
@@ -1890,17 +1890,17 @@
       </c>
       <c r="C31" s="12" t="inlineStr">
         <is>
-          <t>WebView</t>
+          <t>Extra</t>
         </is>
       </c>
       <c r="D31" s="12" t="inlineStr">
         <is>
-          <t>App is using webview</t>
+          <t>App properly configures auto-correction</t>
         </is>
       </c>
       <c r="E31" s="12" t="inlineStr">
         <is>
-          <t>JavaScript is disabled in WebViews unless explicitly required</t>
+          <t>Auto-correction should be disabled for sensitive input</t>
         </is>
       </c>
       <c r="F31" s="12" t="inlineStr"/>
@@ -1922,7 +1922,7 @@
     <row r="32">
       <c r="A32" s="12" t="inlineStr">
         <is>
-          <t>SU.1</t>
+          <t>SW.1</t>
         </is>
       </c>
       <c r="B32" s="12" t="inlineStr">
@@ -1932,17 +1932,17 @@
       </c>
       <c r="C32" s="12" t="inlineStr">
         <is>
-          <t>Upload</t>
+          <t>WebView</t>
         </is>
       </c>
       <c r="D32" s="12" t="inlineStr">
         <is>
-          <t>App has file upload</t>
+          <t>App is using webview</t>
         </is>
       </c>
       <c r="E32" s="12" t="inlineStr">
         <is>
-          <t>Limit maximum number of files that can be uploaded at once</t>
+          <t>JavaScript is disabled in WebViews unless explicitly required</t>
         </is>
       </c>
       <c r="F32" s="12" t="inlineStr"/>
@@ -1964,7 +1964,7 @@
     <row r="33">
       <c r="A33" s="12" t="inlineStr">
         <is>
-          <t>SG.1</t>
+          <t>SU.1</t>
         </is>
       </c>
       <c r="B33" s="12" t="inlineStr">
@@ -1974,17 +1974,17 @@
       </c>
       <c r="C33" s="12" t="inlineStr">
         <is>
-          <t>GDPR</t>
+          <t>Upload</t>
         </is>
       </c>
       <c r="D33" s="12" t="inlineStr">
         <is>
-          <t>Persising user personal information (name, phone, email, ...) on the device</t>
+          <t>App has file upload</t>
         </is>
       </c>
       <c r="E33" s="12" t="inlineStr">
         <is>
-          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
+          <t>Limit maximum number of files that can be uploaded at once</t>
         </is>
       </c>
       <c r="F33" s="12" t="inlineStr"/>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="H33" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I33" s="14" t="inlineStr">
@@ -2006,7 +2006,7 @@
     <row r="34">
       <c r="A34" s="12" t="inlineStr">
         <is>
-          <t>SG.2</t>
+          <t>SG.1</t>
         </is>
       </c>
       <c r="B34" s="12" t="inlineStr">
@@ -2021,12 +2021,12 @@
       </c>
       <c r="D34" s="12" t="inlineStr">
         <is>
-          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
+          <t>Persising user personal information (name, phone, email, ...) on the device</t>
         </is>
       </c>
       <c r="E34" s="12" t="inlineStr">
         <is>
-          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
+          <t>Persisted database should be encrypted when not used. Storage data should not be easily accessible and kept unencrypted</t>
         </is>
       </c>
       <c r="F34" s="12" t="inlineStr"/>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="H34" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I34" s="14" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="35">
       <c r="A35" s="12" t="inlineStr">
         <is>
-          <t>SG.3</t>
+          <t>SG.2</t>
         </is>
       </c>
       <c r="B35" s="12" t="inlineStr">
@@ -2063,12 +2063,12 @@
       </c>
       <c r="D35" s="12" t="inlineStr">
         <is>
-          <t>Sending personal data outside of the application</t>
+          <t>Saving sensitive data in local storage (Keychain, SQLite, ...)</t>
         </is>
       </c>
       <c r="E35" s="12" t="inlineStr">
         <is>
-          <t>All requests must be authenticated</t>
+          <t>The app’s local storage should be wiped after an excessive number of failed authentication attempts</t>
         </is>
       </c>
       <c r="F35" s="12" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="H35" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I35" s="14" t="inlineStr">
@@ -2090,7 +2090,7 @@
     <row r="36">
       <c r="A36" s="12" t="inlineStr">
         <is>
-          <t>SG.4</t>
+          <t>SG.3</t>
         </is>
       </c>
       <c r="B36" s="12" t="inlineStr">
@@ -2105,12 +2105,12 @@
       </c>
       <c r="D36" s="12" t="inlineStr">
         <is>
-          <t>Transferin personal data through REST API</t>
+          <t>Sending personal data outside of the application</t>
         </is>
       </c>
       <c r="E36" s="12" t="inlineStr">
         <is>
-          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
+          <t>All requests must be authenticated</t>
         </is>
       </c>
       <c r="F36" s="12" t="inlineStr"/>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="H36" s="12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I36" s="14" t="inlineStr">
@@ -2132,7 +2132,7 @@
     <row r="37">
       <c r="A37" s="12" t="inlineStr">
         <is>
-          <t>SG.5</t>
+          <t>SG.4</t>
         </is>
       </c>
       <c r="B37" s="12" t="inlineStr">
@@ -2147,12 +2147,12 @@
       </c>
       <c r="D37" s="12" t="inlineStr">
         <is>
-          <t>Displaying privacy policy screen during registration process</t>
+          <t>Transferin personal data through REST API</t>
         </is>
       </c>
       <c r="E37" s="12" t="inlineStr">
         <is>
-          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
+          <t>Certificate pinning should be implemented and HTTPS protocol used for network communication</t>
         </is>
       </c>
       <c r="F37" s="12" t="inlineStr"/>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="H37" s="12" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I37" s="14" t="inlineStr">
@@ -2174,7 +2174,7 @@
     <row r="38">
       <c r="A38" s="12" t="inlineStr">
         <is>
-          <t>SG.6</t>
+          <t>SG.5</t>
         </is>
       </c>
       <c r="B38" s="12" t="inlineStr">
@@ -2189,12 +2189,12 @@
       </c>
       <c r="D38" s="12" t="inlineStr">
         <is>
-          <t>Using non-production environments</t>
+          <t>Displaying privacy policy screen during registration process</t>
         </is>
       </c>
       <c r="E38" s="12" t="inlineStr">
         <is>
-          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
+          <t>The privacy policy must be directly accepted by the user, you can use unchecked checkbox</t>
         </is>
       </c>
       <c r="F38" s="12" t="inlineStr"/>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="H38" s="12" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="I38" s="14" t="inlineStr">
@@ -2216,7 +2216,7 @@
     <row r="39">
       <c r="A39" s="12" t="inlineStr">
         <is>
-          <t>SEM.1</t>
+          <t>SG.6</t>
         </is>
       </c>
       <c r="B39" s="12" t="inlineStr">
@@ -2226,17 +2226,17 @@
       </c>
       <c r="C39" s="12" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>GDPR</t>
         </is>
       </c>
       <c r="D39" s="12" t="inlineStr">
         <is>
-          <t>Application has input for user email address</t>
+          <t>Using non-production environments</t>
         </is>
       </c>
       <c r="E39" s="12" t="inlineStr">
         <is>
-          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
+          <t>Non-production environments (development, staging, beta) **can not** contain any real personal data</t>
         </is>
       </c>
       <c r="F39" s="12" t="inlineStr"/>
@@ -2258,7 +2258,7 @@
     <row r="40">
       <c r="A40" s="12" t="inlineStr">
         <is>
-          <t>SV.1</t>
+          <t>SEM.1</t>
         </is>
       </c>
       <c r="B40" s="12" t="inlineStr">
@@ -2268,17 +2268,17 @@
       </c>
       <c r="C40" s="12" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="D40" s="12" t="inlineStr">
         <is>
-          <t>User can play video in the application</t>
+          <t>Application has input for user email address</t>
         </is>
       </c>
       <c r="E40" s="12" t="inlineStr">
         <is>
-          <t>Video data must be received through encrypted protocol</t>
+          <t>Email input should be validated and limited in maximum characters to e.g. 100 characters</t>
         </is>
       </c>
       <c r="F40" s="12" t="inlineStr"/>
@@ -2300,7 +2300,7 @@
     <row r="41">
       <c r="A41" s="12" t="inlineStr">
         <is>
-          <t>SL.1</t>
+          <t>SV.1</t>
         </is>
       </c>
       <c r="B41" s="12" t="inlineStr">
@@ -2310,17 +2310,17 @@
       </c>
       <c r="C41" s="12" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="D41" s="12" t="inlineStr">
         <is>
-          <t>App is using location services</t>
+          <t>User can play video in the application</t>
         </is>
       </c>
       <c r="E41" s="12" t="inlineStr">
         <is>
-          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+          <t>Video data must be received through encrypted protocol</t>
         </is>
       </c>
       <c r="F41" s="12" t="inlineStr"/>
@@ -2330,17 +2330,59 @@
       </c>
       <c r="H41" s="12" t="inlineStr">
         <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I41" s="14" t="inlineStr">
+        <is>
+          <t>Handbook</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="12" t="inlineStr">
+        <is>
+          <t>SL.1</t>
+        </is>
+      </c>
+      <c r="B42" s="12" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="C42" s="12" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D42" s="12" t="inlineStr">
+        <is>
+          <t>App is using location services</t>
+        </is>
+      </c>
+      <c r="E42" s="12" t="inlineStr">
+        <is>
+          <t>Detect mocked location and let user know. Also check how it's affecting app and should it be possible to fake location</t>
+        </is>
+      </c>
+      <c r="F42" s="12" t="inlineStr"/>
+      <c r="G42" s="13">
+        <f>IFERROR(B42+F4242+"x",TODAY())</f>
+        <v/>
+      </c>
+      <c r="H42" s="12" t="inlineStr">
+        <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I41" s="14" t="inlineStr">
+      <c r="I42" s="14" t="inlineStr">
         <is>
           <t>Handbook</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C41"/>
+  <autoFilter ref="C1:C42"/>
   <conditionalFormatting sqref="A2:I980">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>$B2="TODO"</formula>
@@ -2356,10 +2398,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38 B39 B40 B41" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21 B22 B23 B24 B25 B26 B27 B28 B29 B30 B31 B32 B33 B34 B35 B36 B37 B38 B39 B40 B41 B42" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"TODO,DONE,Won't fix,Not applicable"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40 H41" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40 H41 H42" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"Critical,High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2404,6 +2446,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I39" r:id="rId38"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I40" r:id="rId39"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I41" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I42" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>